<commit_message>
Planning en unity folder
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
   <si>
     <t>Satyr</t>
   </si>
@@ -319,13 +319,25 @@
   </si>
   <si>
     <t>Week 27</t>
+  </si>
+  <si>
+    <t>Player Controller</t>
+  </si>
+  <si>
+    <t>Camera Controller</t>
+  </si>
+  <si>
+    <t>Scripts</t>
+  </si>
+  <si>
+    <t>Particles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,14 +351,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,6 +419,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -441,29 +459,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -783,75 +798,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:9" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="15" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -869,14 +878,15 @@
       <c r="G4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="14"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="15" t="s">
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -894,14 +904,15 @@
       <c r="G5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="14"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="15" t="s">
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13"/>
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -919,14 +930,15 @@
       <c r="G6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="15" t="s">
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13"/>
+      <c r="B7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -938,16 +950,17 @@
       <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
       <c r="I7" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="15" t="s">
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -959,16 +972,17 @@
       <c r="E8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
       <c r="I8" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="15" t="s">
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -980,226 +994,308 @@
       <c r="E9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
       <c r="I9" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="J11" s="17"/>
+    </row>
+    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="13"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17" t="s">
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15" t="s">
         <v>71</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
       <c r="B13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13"/>
       <c r="B14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13"/>
       <c r="B15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17" t="s">
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
       <c r="B16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="17" t="s">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
       <c r="B17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
       <c r="B18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17" t="s">
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="J18" s="17"/>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
       <c r="B19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="3"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="3"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="15"/>
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="15"/>
+      <c r="J20" s="17"/>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="13"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="15"/>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="J23" s="17"/>
+    </row>
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="13"/>
+      <c r="J24" s="17"/>
+    </row>
+    <row r="25" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J25" s="17"/>
+    </row>
+    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="15"/>
+      <c r="J28" s="17"/>
+    </row>
+    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="17"/>
+      <c r="B29" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H29" s="15"/>
+      <c r="I29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="17"/>
+    </row>
+    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="17"/>
+      <c r="B30" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" s="15"/>
+      <c r="I30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="17"/>
+    </row>
+    <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="17"/>
+      <c r="H31" s="15"/>
+      <c r="J31" s="17"/>
+    </row>
+    <row r="32" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J33" s="17"/>
+    </row>
+    <row r="34" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J34" s="17"/>
+    </row>
+    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="15"/>
+      <c r="J35" s="17"/>
+    </row>
+    <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="17"/>
+      <c r="H36" s="15"/>
+      <c r="J36" s="17"/>
+    </row>
+    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17"/>
+      <c r="H37" s="15"/>
+      <c r="J37" s="17"/>
+    </row>
+    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="17"/>
+      <c r="H38" s="15"/>
+      <c r="J38" s="17"/>
+    </row>
+    <row r="39" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1211,70 +1307,70 @@
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" style="19" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="4" customWidth="1"/>
     <col min="9" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3" style="19" customWidth="1"/>
+    <col min="11" max="11" width="3" style="4" customWidth="1"/>
     <col min="12" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.85546875" style="19" customWidth="1"/>
+    <col min="14" max="14" width="2.85546875" style="4" customWidth="1"/>
     <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="2.85546875" style="19" customWidth="1"/>
+    <col min="19" max="19" width="2.85546875" style="4" customWidth="1"/>
     <col min="20" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="2.85546875" style="19" customWidth="1"/>
+    <col min="22" max="22" width="2.85546875" style="4" customWidth="1"/>
     <col min="23" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="2.85546875" style="19" customWidth="1"/>
+    <col min="25" max="25" width="2.85546875" style="4" customWidth="1"/>
     <col min="26" max="27" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="2.85546875" style="19" customWidth="1"/>
+    <col min="28" max="28" width="2.85546875" style="4" customWidth="1"/>
     <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="20"/>
+      <c r="B1" s="5"/>
       <c r="C1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="20"/>
+      <c r="E1" s="5"/>
       <c r="F1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="20"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="1" t="s">
         <v>81</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="20"/>
+      <c r="K1" s="5"/>
       <c r="L1" s="1" t="s">
         <v>83</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="20"/>
+      <c r="N1" s="5"/>
       <c r="O1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="6" t="s">
         <v>86</v>
       </c>
       <c r="Q1" s="1" t="s">
@@ -1283,392 +1379,392 @@
       <c r="R1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="20"/>
+      <c r="S1" s="5"/>
       <c r="T1" s="1" t="s">
         <v>88</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="V1" s="20"/>
+      <c r="V1" s="5"/>
       <c r="W1" s="1" t="s">
         <v>93</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Y1" s="20"/>
+      <c r="Y1" s="5"/>
       <c r="Z1" s="1" t="s">
         <v>95</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AB1" s="20"/>
+      <c r="AB1" s="5"/>
       <c r="AC1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AD1" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AD2" s="21"/>
+    <row r="2" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AD2" s="6"/>
     </row>
     <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="P3" s="21"/>
-      <c r="S3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="AB3" s="20"/>
-      <c r="AD3" s="21"/>
+      <c r="B3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="P3" s="6"/>
+      <c r="S3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AD3" s="6"/>
     </row>
     <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="P4" s="21"/>
-      <c r="S4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="AB4" s="20"/>
-      <c r="AD4" s="21"/>
+      <c r="B4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="P4" s="6"/>
+      <c r="S4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AD4" s="6"/>
     </row>
     <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="P5" s="21"/>
-      <c r="S5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="Y5" s="20"/>
-      <c r="AB5" s="20"/>
-      <c r="AD5" s="21"/>
+      <c r="B5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="S5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AD5" s="6"/>
     </row>
     <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="P6" s="21"/>
-      <c r="S6" s="20"/>
-      <c r="V6" s="20"/>
-      <c r="Y6" s="20"/>
-      <c r="AB6" s="20"/>
-      <c r="AD6" s="21"/>
+      <c r="B6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="P6" s="6"/>
+      <c r="S6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AD6" s="6"/>
     </row>
     <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="P7" s="21"/>
-      <c r="S7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="Y7" s="20"/>
-      <c r="AB7" s="20"/>
-      <c r="AD7" s="21"/>
-    </row>
-    <row r="8" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AD8" s="21"/>
+      <c r="B7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="P7" s="6"/>
+      <c r="S7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AD7" s="6"/>
+    </row>
+    <row r="8" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AD8" s="6"/>
     </row>
     <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="P9" s="21"/>
-      <c r="S9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="Y9" s="20"/>
-      <c r="AB9" s="20"/>
-      <c r="AD9" s="21"/>
+      <c r="B9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="P9" s="6"/>
+      <c r="S9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AD9" s="6"/>
     </row>
     <row r="10" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="P10" s="21"/>
-      <c r="S10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="Y10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AD10" s="21"/>
+      <c r="B10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="P10" s="6"/>
+      <c r="S10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AD10" s="6"/>
     </row>
     <row r="11" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="P11" s="21"/>
-      <c r="S11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="Y11" s="20"/>
-      <c r="AB11" s="20"/>
-      <c r="AD11" s="21"/>
+      <c r="B11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="P11" s="6"/>
+      <c r="S11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AD11" s="6"/>
     </row>
     <row r="12" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="P12" s="21"/>
-      <c r="S12" s="20"/>
-      <c r="V12" s="20"/>
-      <c r="Y12" s="20"/>
-      <c r="AB12" s="20"/>
-      <c r="AD12" s="21"/>
+      <c r="B12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="P12" s="6"/>
+      <c r="S12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="AB12" s="5"/>
+      <c r="AD12" s="6"/>
     </row>
     <row r="13" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="P13" s="21"/>
-      <c r="S13" s="20"/>
-      <c r="V13" s="20"/>
-      <c r="Y13" s="20"/>
-      <c r="AB13" s="20"/>
-      <c r="AD13" s="21"/>
-    </row>
-    <row r="14" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AD14" s="21"/>
+      <c r="B13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="P13" s="6"/>
+      <c r="S13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AD13" s="6"/>
+    </row>
+    <row r="14" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AD14" s="6"/>
     </row>
     <row r="15" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="P15" s="21"/>
-      <c r="S15" s="20"/>
-      <c r="V15" s="20"/>
-      <c r="Y15" s="20"/>
-      <c r="AB15" s="20"/>
-      <c r="AD15" s="21"/>
+      <c r="B15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="P15" s="6"/>
+      <c r="S15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AD15" s="6"/>
     </row>
     <row r="16" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="P16" s="21"/>
-      <c r="S16" s="20"/>
-      <c r="V16" s="20"/>
-      <c r="Y16" s="20"/>
-      <c r="AB16" s="20"/>
-      <c r="AD16" s="21"/>
+      <c r="B16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="P16" s="6"/>
+      <c r="S16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AD16" s="6"/>
     </row>
     <row r="17" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="P17" s="21"/>
-      <c r="S17" s="20"/>
-      <c r="V17" s="20"/>
-      <c r="Y17" s="20"/>
-      <c r="AB17" s="20"/>
-      <c r="AD17" s="21"/>
+      <c r="B17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="P17" s="6"/>
+      <c r="S17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AD17" s="6"/>
     </row>
     <row r="18" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="P18" s="21"/>
-      <c r="S18" s="20"/>
-      <c r="V18" s="20"/>
-      <c r="Y18" s="20"/>
-      <c r="AB18" s="20"/>
-      <c r="AD18" s="21"/>
+      <c r="B18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="P18" s="6"/>
+      <c r="S18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AD18" s="6"/>
     </row>
     <row r="19" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="P19" s="21"/>
-      <c r="S19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="Y19" s="20"/>
-      <c r="AB19" s="20"/>
-      <c r="AD19" s="21"/>
-    </row>
-    <row r="20" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AD20" s="21"/>
+      <c r="B19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="P19" s="6"/>
+      <c r="S19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AD19" s="6"/>
+    </row>
+    <row r="20" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AD20" s="6"/>
     </row>
     <row r="21" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="P21" s="21"/>
-      <c r="S21" s="20"/>
-      <c r="V21" s="20"/>
-      <c r="Y21" s="20"/>
-      <c r="AB21" s="20"/>
-      <c r="AD21" s="21"/>
+      <c r="B21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="P21" s="6"/>
+      <c r="S21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AD21" s="6"/>
     </row>
     <row r="22" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="P22" s="21"/>
-      <c r="S22" s="20"/>
-      <c r="V22" s="20"/>
-      <c r="Y22" s="20"/>
-      <c r="AB22" s="20"/>
-      <c r="AD22" s="21"/>
+      <c r="B22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="P22" s="6"/>
+      <c r="S22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AD22" s="6"/>
     </row>
     <row r="23" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="P23" s="21"/>
-      <c r="S23" s="20"/>
-      <c r="V23" s="20"/>
-      <c r="Y23" s="20"/>
-      <c r="AB23" s="20"/>
-      <c r="AD23" s="21"/>
+      <c r="B23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="P23" s="6"/>
+      <c r="S23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AD23" s="6"/>
     </row>
     <row r="24" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="P24" s="21"/>
-      <c r="S24" s="20"/>
-      <c r="V24" s="20"/>
-      <c r="Y24" s="20"/>
-      <c r="AB24" s="20"/>
-      <c r="AD24" s="21"/>
+      <c r="B24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="P24" s="6"/>
+      <c r="S24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="AB24" s="5"/>
+      <c r="AD24" s="6"/>
     </row>
     <row r="25" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="P25" s="21"/>
-      <c r="S25" s="20"/>
-      <c r="V25" s="20"/>
-      <c r="Y25" s="20"/>
-      <c r="AB25" s="20"/>
-      <c r="AD25" s="21"/>
-    </row>
-    <row r="26" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AD26" s="21"/>
+      <c r="B25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="P25" s="6"/>
+      <c r="S25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="AB25" s="5"/>
+      <c r="AD25" s="6"/>
+    </row>
+    <row r="26" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AD26" s="6"/>
     </row>
     <row r="27" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="P27" s="21"/>
-      <c r="S27" s="20"/>
-      <c r="V27" s="20"/>
-      <c r="Y27" s="20"/>
-      <c r="AB27" s="20"/>
-      <c r="AD27" s="21"/>
+      <c r="B27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="P27" s="6"/>
+      <c r="S27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AD27" s="6"/>
     </row>
     <row r="28" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="P28" s="21"/>
-      <c r="S28" s="20"/>
-      <c r="V28" s="20"/>
-      <c r="Y28" s="20"/>
-      <c r="AB28" s="20"/>
-      <c r="AD28" s="21"/>
+      <c r="B28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="P28" s="6"/>
+      <c r="S28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AD28" s="6"/>
     </row>
     <row r="29" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="P29" s="21"/>
-      <c r="S29" s="20"/>
-      <c r="V29" s="20"/>
-      <c r="Y29" s="20"/>
-      <c r="AB29" s="20"/>
-      <c r="AD29" s="21"/>
+      <c r="B29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="P29" s="6"/>
+      <c r="S29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="AB29" s="5"/>
+      <c r="AD29" s="6"/>
     </row>
     <row r="30" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="P30" s="21"/>
-      <c r="S30" s="20"/>
-      <c r="V30" s="20"/>
-      <c r="Y30" s="20"/>
-      <c r="AB30" s="20"/>
-      <c r="AD30" s="21"/>
+      <c r="B30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="P30" s="6"/>
+      <c r="S30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AD30" s="6"/>
     </row>
     <row r="31" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="P31" s="21"/>
-      <c r="S31" s="20"/>
-      <c r="V31" s="20"/>
-      <c r="Y31" s="20"/>
-      <c r="AB31" s="20"/>
-      <c r="AD31" s="21"/>
-    </row>
-    <row r="32" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AD32" s="21"/>
+      <c r="B31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="P31" s="6"/>
+      <c r="S31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="AB31" s="5"/>
+      <c r="AD31" s="6"/>
+    </row>
+    <row r="32" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AD32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Assetlist, planning en graphic concept
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
   <si>
     <t>Satyr</t>
   </si>
@@ -331,6 +331,51 @@
   </si>
   <si>
     <t>Particles</t>
+  </si>
+  <si>
+    <t>HUD</t>
+  </si>
+  <si>
+    <t>Health bar outline</t>
+  </si>
+  <si>
+    <t>Health bar</t>
+  </si>
+  <si>
+    <t>Experience bar outline</t>
+  </si>
+  <si>
+    <t>Experience bar</t>
+  </si>
+  <si>
+    <t>Ability button</t>
+  </si>
+  <si>
+    <t>Ability button pressed</t>
+  </si>
+  <si>
+    <t>Font</t>
+  </si>
+  <si>
+    <t>2D_HUD_HPOUTLINE</t>
+  </si>
+  <si>
+    <t>2D_HUD_HPBAR</t>
+  </si>
+  <si>
+    <t>2D_HUD_XPOUTLINE</t>
+  </si>
+  <si>
+    <t>2D_HUD_XPBAR</t>
+  </si>
+  <si>
+    <t>2D_HUD_ABILITYPRESS</t>
+  </si>
+  <si>
+    <t>2D_HUD_FONT</t>
+  </si>
+  <si>
+    <t>2D_HUD_ABILITY</t>
   </si>
 </sst>
 </file>
@@ -459,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -479,6 +524,8 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -798,17 +845,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.5703125" bestFit="1" customWidth="1"/>
@@ -855,7 +903,8 @@
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
       <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1015,7 +1064,8 @@
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
       <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1205,27 +1255,42 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
       <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="J24" s="17"/>
     </row>
-    <row r="25" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13"/>
       <c r="J25" s="17"/>
     </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+    <row r="28" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="17"/>
+      <c r="B28" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>110</v>
+      </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
@@ -1233,69 +1298,181 @@
       <c r="H28" s="15"/>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="B29" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
-      <c r="B30" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="B30" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
       <c r="H30" s="15"/>
-      <c r="I30" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
+      <c r="B31" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
       <c r="H31" s="15"/>
       <c r="J31" s="17"/>
     </row>
-    <row r="32" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="17"/>
+      <c r="B32" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="15"/>
+      <c r="J32" s="17"/>
+    </row>
+    <row r="33" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="17"/>
+      <c r="B33" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="15"/>
       <c r="J33" s="17"/>
     </row>
-    <row r="34" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="17"/>
+      <c r="B34" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="15"/>
       <c r="J34" s="17"/>
     </row>
-    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J36" s="17"/>
+    </row>
+    <row r="37" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J37" s="17"/>
+    </row>
+    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="17"/>
+    </row>
+    <row r="39" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="17"/>
+      <c r="B39" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H39" s="15"/>
+      <c r="I39" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J39" s="17"/>
+    </row>
+    <row r="40" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="17"/>
+      <c r="B40" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H40" s="15"/>
+      <c r="I40" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J40" s="17"/>
+    </row>
+    <row r="41" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="17"/>
+      <c r="H41" s="15"/>
+      <c r="J41" s="17"/>
+    </row>
+    <row r="42" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J43" s="17"/>
+    </row>
+    <row r="44" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J44" s="17"/>
+    </row>
+    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="15"/>
-      <c r="J35" s="17"/>
-    </row>
-    <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
-      <c r="H36" s="15"/>
-      <c r="J36" s="17"/>
-    </row>
-    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
-      <c r="H37" s="15"/>
-      <c r="J37" s="17"/>
-    </row>
-    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="H38" s="15"/>
-      <c r="J38" s="17"/>
-    </row>
-    <row r="39" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="17"/>
+    </row>
+    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="17"/>
+      <c r="H46" s="15"/>
+      <c r="J46" s="17"/>
+    </row>
+    <row r="47" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="17"/>
+      <c r="H47" s="15"/>
+      <c r="J47" s="17"/>
+    </row>
+    <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="17"/>
+      <c r="H48" s="15"/>
+      <c r="J48" s="17"/>
+    </row>
+    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1307,15 +1484,15 @@
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.85546875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" style="4" customWidth="1"/>
@@ -1416,6 +1593,9 @@
         <v>90</v>
       </c>
       <c r="B3" s="5"/>
+      <c r="C3" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="H3" s="5"/>
       <c r="K3" s="5"/>
@@ -1429,6 +1609,9 @@
     </row>
     <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
+      <c r="C4" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
       <c r="K4" s="5"/>
@@ -1629,6 +1812,9 @@
         <v>37</v>
       </c>
       <c r="B21" s="5"/>
+      <c r="C21" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="H21" s="5"/>
       <c r="K21" s="5"/>
@@ -1642,6 +1828,9 @@
     </row>
     <row r="22" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
+      <c r="C22" s="20" t="s">
+        <v>35</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="H22" s="5"/>
       <c r="K22" s="5"/>
@@ -1655,6 +1844,9 @@
     </row>
     <row r="23" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
+      <c r="C23" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="H23" s="5"/>
       <c r="K23" s="5"/>

</xml_diff>

<commit_message>
Planning and gdd update
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="141">
   <si>
     <t>Satyr</t>
   </si>
@@ -376,6 +376,78 @@
   </si>
   <si>
     <t>2D_HUD_ABILITY</t>
+  </si>
+  <si>
+    <t>Flower Plant</t>
+  </si>
+  <si>
+    <t>Seaweed</t>
+  </si>
+  <si>
+    <t>2D_ENV_FLOWER</t>
+  </si>
+  <si>
+    <t>2D_ENV_SEAWEED</t>
+  </si>
+  <si>
+    <t>3D_ENV_FLOWER</t>
+  </si>
+  <si>
+    <t>UW_ENV_FLOWER</t>
+  </si>
+  <si>
+    <t>3D_ENV_SEAWEED</t>
+  </si>
+  <si>
+    <t>UW_ENV_SEAWEED</t>
+  </si>
+  <si>
+    <t>Helmet</t>
+  </si>
+  <si>
+    <t>Chest plate</t>
+  </si>
+  <si>
+    <t>Arm guards</t>
+  </si>
+  <si>
+    <t>Boots of Hermes</t>
+  </si>
+  <si>
+    <t>2D_PROP_HELMET</t>
+  </si>
+  <si>
+    <t>3D_PROP_HELMET</t>
+  </si>
+  <si>
+    <t>UW_PROP_HELMET</t>
+  </si>
+  <si>
+    <t>2D_PROP_CHEST</t>
+  </si>
+  <si>
+    <t>3D_PROP_CHEST</t>
+  </si>
+  <si>
+    <t>UW_PROP_CHEST</t>
+  </si>
+  <si>
+    <t>2D_PROP_GUARDS</t>
+  </si>
+  <si>
+    <t>3D_PROP_GUARDS</t>
+  </si>
+  <si>
+    <t>UW_PROP_GUARDS</t>
+  </si>
+  <si>
+    <t>2D_PROP_BOOTS</t>
+  </si>
+  <si>
+    <t>3D_PROP_BOOTS</t>
+  </si>
+  <si>
+    <t>UW_PROP_BOOTS</t>
   </si>
 </sst>
 </file>
@@ -477,7 +549,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -500,11 +572,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -526,6 +609,8 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -845,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,6 +1194,9 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
+      <c r="I13" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1128,6 +1216,9 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="15"/>
+      <c r="I14" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1145,6 +1236,9 @@
       <c r="H15" s="15" t="s">
         <v>72</v>
       </c>
+      <c r="I15" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1166,6 +1260,9 @@
       <c r="H16" s="15" t="s">
         <v>54</v>
       </c>
+      <c r="I16" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1185,6 +1282,9 @@
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
+      <c r="I17" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="J17" s="17"/>
     </row>
     <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1206,6 +1306,9 @@
       <c r="H18" s="15" t="s">
         <v>54</v>
       </c>
+      <c r="I18" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="J18" s="17"/>
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1225,146 +1328,205 @@
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="15"/>
+      <c r="I19" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="J19" s="17"/>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
+      <c r="B20" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
+      <c r="I20" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
+      <c r="B21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
+      <c r="I21" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="J21" s="17"/>
     </row>
-    <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
       <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="A23" s="13"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
+      <c r="H23" s="15"/>
       <c r="J23" s="17"/>
     </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
+    <row r="24" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
+      <c r="A25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
       <c r="J25" s="17"/>
     </row>
-    <row r="26" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13"/>
+      <c r="B26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13"/>
+      <c r="B27" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="13"/>
+      <c r="B28" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
+      <c r="I28" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13"/>
+      <c r="B29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="15"/>
+      <c r="I29" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="15"/>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-      <c r="B31" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="15"/>
+    <row r="31" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
-      <c r="B32" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>116</v>
-      </c>
+      <c r="A32" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
       <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="19" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
@@ -1376,10 +1538,10 @@
     <row r="34" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
@@ -1388,73 +1550,122 @@
       <c r="H34" s="15"/>
       <c r="J34" s="17"/>
     </row>
-    <row r="35" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="17"/>
+      <c r="B35" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="15"/>
+      <c r="J35" s="17"/>
+    </row>
+    <row r="36" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="17"/>
+      <c r="B36" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="15"/>
       <c r="J36" s="17"/>
     </row>
-    <row r="37" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17"/>
+      <c r="B37" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="15"/>
       <c r="J37" s="17"/>
     </row>
-    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+    <row r="38" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="17"/>
+      <c r="B38" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>114</v>
+      </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
+      <c r="H38" s="15"/>
       <c r="J38" s="17"/>
     </row>
-    <row r="39" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="15"/>
+      <c r="J39" s="17"/>
+    </row>
+    <row r="40" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J41" s="17"/>
+    </row>
+    <row r="42" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J42" s="17"/>
+    </row>
+    <row r="43" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="17"/>
+    </row>
+    <row r="44" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="17"/>
+      <c r="B44" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H39" s="15"/>
-      <c r="I39" s="3" t="s">
+      <c r="H44" s="15"/>
+      <c r="I44" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J39" s="17"/>
-    </row>
-    <row r="40" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
-      <c r="B40" s="3" t="s">
+      <c r="J44" s="17"/>
+    </row>
+    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="17"/>
+      <c r="B45" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H40" s="15"/>
-      <c r="I40" s="3" t="s">
+      <c r="H45" s="15"/>
+      <c r="I45" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J40" s="17"/>
-    </row>
-    <row r="41" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
-      <c r="H41" s="15"/>
-      <c r="J41" s="17"/>
-    </row>
-    <row r="42" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J43" s="17"/>
-    </row>
-    <row r="44" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J44" s="17"/>
-    </row>
-    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
       <c r="J45" s="17"/>
     </row>
     <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1462,17 +1673,43 @@
       <c r="H46" s="15"/>
       <c r="J46" s="17"/>
     </row>
-    <row r="47" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
-      <c r="H47" s="15"/>
-      <c r="J47" s="17"/>
-    </row>
+    <row r="47" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
-      <c r="H48" s="15"/>
       <c r="J48" s="17"/>
     </row>
-    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J49" s="17"/>
+    </row>
+    <row r="50" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="17"/>
+    </row>
+    <row r="51" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="17"/>
+      <c r="H51" s="15"/>
+      <c r="J51" s="17"/>
+    </row>
+    <row r="52" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="17"/>
+      <c r="H52" s="15"/>
+      <c r="J52" s="17"/>
+    </row>
+    <row r="53" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="17"/>
+      <c r="H53" s="15"/>
+      <c r="J53" s="17"/>
+    </row>
+    <row r="54" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1483,24 +1720,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.85546875" style="4" customWidth="1"/>
-    <col min="6" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" style="4" customWidth="1"/>
-    <col min="9" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" style="4" customWidth="1"/>
-    <col min="12" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2.85546875" style="4" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2.85546875" style="4" customWidth="1"/>
@@ -1892,10 +2130,37 @@
         <v>30</v>
       </c>
       <c r="B27" s="5"/>
+      <c r="C27" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="E27" s="5"/>
+      <c r="F27" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>20</v>
+      </c>
       <c r="H27" s="5"/>
-      <c r="K27" s="5"/>
+      <c r="I27" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K27" s="21"/>
+      <c r="L27" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" s="22" t="s">
+        <v>14</v>
+      </c>
       <c r="N27" s="5"/>
+      <c r="O27" s="22" t="s">
+        <v>17</v>
+      </c>
       <c r="P27" s="6"/>
       <c r="S27" s="5"/>
       <c r="V27" s="5"/>
@@ -1905,9 +2170,28 @@
     </row>
     <row r="28" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
+      <c r="C28" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="E28" s="5"/>
+      <c r="F28" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="H28" s="5"/>
+      <c r="I28" s="22"/>
       <c r="K28" s="5"/>
+      <c r="L28" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" s="22" t="s">
+        <v>16</v>
+      </c>
       <c r="N28" s="5"/>
       <c r="P28" s="6"/>
       <c r="S28" s="5"/>

</xml_diff>

<commit_message>
Assetlist update. Player controller almost done and experience manager as good as done
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="157">
   <si>
     <t>Satyr</t>
   </si>
@@ -448,6 +448,54 @@
   </si>
   <si>
     <t>UW_PROP_BOOTS</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Enemies</t>
+  </si>
+  <si>
+    <t>Game manager</t>
+  </si>
+  <si>
+    <t>Quest manager</t>
+  </si>
+  <si>
+    <t>Pause manager</t>
+  </si>
+  <si>
+    <t>Main menu manager</t>
+  </si>
+  <si>
+    <t>Load manager</t>
+  </si>
+  <si>
+    <t>Options manager</t>
+  </si>
+  <si>
+    <t>Experience manager</t>
+  </si>
+  <si>
+    <t>Crafting</t>
+  </si>
+  <si>
+    <t>Satyr behavior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minotaur behavior </t>
+  </si>
+  <si>
+    <t>UI manager</t>
+  </si>
+  <si>
+    <t>Pick ups</t>
+  </si>
+  <si>
+    <t>Craftables</t>
   </si>
 </sst>
 </file>
@@ -469,7 +517,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,6 +596,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -587,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -611,6 +665,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -930,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H58" activeCellId="1" sqref="H44 H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,21 +1701,17 @@
       <c r="I43" s="14"/>
       <c r="J43" s="17"/>
     </row>
-    <row r="44" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="B44" s="3" t="s">
-        <v>98</v>
+    <row r="44" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="23" t="s">
+        <v>141</v>
       </c>
       <c r="H44" s="15"/>
-      <c r="I44" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="J44" s="17"/>
     </row>
     <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H45" s="15"/>
       <c r="I45" s="3" t="s">
@@ -1670,46 +1721,191 @@
     </row>
     <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
+      <c r="B46" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="H46" s="15"/>
+      <c r="I46" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="J46" s="17"/>
     </row>
-    <row r="47" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="17"/>
+      <c r="B47" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H47" s="15"/>
+      <c r="I47" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J47" s="17"/>
+    </row>
     <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="17"/>
+      <c r="H48" s="15"/>
       <c r="J48" s="17"/>
     </row>
-    <row r="49" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H49" s="15"/>
       <c r="J49" s="17"/>
     </row>
     <row r="50" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H50" s="15"/>
       <c r="J50" s="17"/>
     </row>
     <row r="51" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
+      <c r="B51" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="H51" s="15"/>
       <c r="J51" s="17"/>
     </row>
     <row r="52" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
+      <c r="B52" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="H52" s="15"/>
       <c r="J52" s="17"/>
     </row>
     <row r="53" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
+      <c r="B53" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="H53" s="15"/>
       <c r="J53" s="17"/>
     </row>
-    <row r="54" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="17"/>
+      <c r="B54" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H54" s="15"/>
+      <c r="J54" s="17"/>
+    </row>
+    <row r="55" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="17"/>
+      <c r="B55" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H55" s="15"/>
+      <c r="J55" s="17"/>
+    </row>
+    <row r="56" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="17"/>
+      <c r="B56" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H56" s="15"/>
+      <c r="I56" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J56" s="17"/>
+    </row>
+    <row r="57" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="17"/>
+      <c r="B57" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H57" s="15"/>
+      <c r="I57" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J57" s="17"/>
+    </row>
+    <row r="58" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="H58" s="15"/>
+      <c r="J58" s="17"/>
+    </row>
+    <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="17"/>
+      <c r="B59" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H59" s="15"/>
+      <c r="J59" s="17"/>
+    </row>
+    <row r="60" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="17"/>
+      <c r="B60" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H60" s="15"/>
+      <c r="J60" s="17"/>
+    </row>
+    <row r="61" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H61" s="15"/>
+      <c r="J61" s="17"/>
+    </row>
+    <row r="62" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="17"/>
+      <c r="B62" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H62" s="15"/>
+      <c r="J62" s="17"/>
+    </row>
+    <row r="63" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="17"/>
+      <c r="B63" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H63" s="15"/>
+      <c r="J63" s="17"/>
+    </row>
+    <row r="64" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J65" s="17"/>
+    </row>
+    <row r="66" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J66" s="17"/>
+    </row>
+    <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="17"/>
+    </row>
+    <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="17"/>
+      <c r="H68" s="15"/>
+      <c r="J68" s="17"/>
+    </row>
+    <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="17"/>
+      <c r="H69" s="15"/>
+      <c r="J69" s="17"/>
+    </row>
+    <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="17"/>
+      <c r="H70" s="15"/>
+      <c r="J70" s="17"/>
+    </row>
+    <row r="71" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1721,7 +1917,7 @@
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,6 +2059,9 @@
     </row>
     <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
+      <c r="C5" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
       <c r="K5" s="5"/>

</xml_diff>

<commit_message>
Pause manager and main menu manager
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="158">
   <si>
     <t>Satyr</t>
   </si>
@@ -991,7 +991,7 @@
   <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,6 +1778,9 @@
         <v>146</v>
       </c>
       <c r="H52" s="15"/>
+      <c r="I52" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="J52" s="17"/>
     </row>
     <row r="53" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1786,6 +1789,9 @@
         <v>147</v>
       </c>
       <c r="H53" s="15"/>
+      <c r="I53" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="J53" s="17"/>
     </row>
     <row r="54" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Gdd + assetlist update. respawn manager and set respawn point
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="163">
   <si>
     <t>Satyr</t>
   </si>
@@ -499,6 +499,21 @@
   </si>
   <si>
     <t>Satyr Spawn</t>
+  </si>
+  <si>
+    <t>Pause Manager</t>
+  </si>
+  <si>
+    <t>Main menu Manager</t>
+  </si>
+  <si>
+    <t>Player respawn manager</t>
+  </si>
+  <si>
+    <t>Set respawn position</t>
+  </si>
+  <si>
+    <t>Set respawn point</t>
   </si>
 </sst>
 </file>
@@ -988,16 +1003,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="26.140625" bestFit="1" customWidth="1"/>
@@ -1835,39 +1850,36 @@
       </c>
       <c r="J57" s="17"/>
     </row>
-    <row r="58" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="23" t="s">
-        <v>143</v>
+    <row r="58" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="17"/>
+      <c r="B58" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="H58" s="15"/>
+      <c r="I58" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="J58" s="17"/>
     </row>
     <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="17"/>
       <c r="B59" s="3" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="H59" s="15"/>
-      <c r="I59" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="J59" s="17"/>
     </row>
-    <row r="60" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="17"/>
-      <c r="B60" s="3" t="s">
-        <v>153</v>
+    <row r="60" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="23" t="s">
+        <v>143</v>
       </c>
       <c r="H60" s="15"/>
-      <c r="I60" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="J60" s="17"/>
     </row>
     <row r="61" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="17"/>
       <c r="B61" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H61" s="15"/>
       <c r="I61" s="3" t="s">
@@ -1876,57 +1888,69 @@
       <c r="J61" s="17"/>
     </row>
     <row r="62" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="23" t="s">
-        <v>31</v>
+      <c r="A62" s="17"/>
+      <c r="B62" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="H62" s="15"/>
+      <c r="I62" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="J62" s="17"/>
     </row>
     <row r="63" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17"/>
       <c r="B63" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H63" s="15"/>
+      <c r="I63" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="J63" s="17"/>
     </row>
     <row r="64" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="17"/>
-      <c r="B64" s="3" t="s">
-        <v>156</v>
+      <c r="A64" s="23" t="s">
+        <v>31</v>
       </c>
       <c r="H64" s="15"/>
       <c r="J64" s="17"/>
     </row>
-    <row r="65" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="17"/>
+      <c r="B65" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H65" s="15"/>
+      <c r="J65" s="17"/>
+    </row>
     <row r="66" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="17"/>
+      <c r="B66" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H66" s="15"/>
       <c r="J66" s="17"/>
     </row>
-    <row r="67" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J67" s="17"/>
-    </row>
+    <row r="67" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+      <c r="J68" s="17"/>
+    </row>
+    <row r="69" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J69" s="17"/>
+    </row>
+    <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="17"/>
-    </row>
-    <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="17"/>
-      <c r="H69" s="15"/>
-      <c r="J69" s="17"/>
-    </row>
-    <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="17"/>
-      <c r="H70" s="15"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
       <c r="J70" s="17"/>
     </row>
     <row r="71" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1934,7 +1958,17 @@
       <c r="H71" s="15"/>
       <c r="J71" s="17"/>
     </row>
-    <row r="72" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="17"/>
+      <c r="H72" s="15"/>
+      <c r="J72" s="17"/>
+    </row>
+    <row r="73" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="17"/>
+      <c r="H73" s="15"/>
+      <c r="J73" s="17"/>
+    </row>
+    <row r="74" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1943,17 +1977,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD32"/>
+  <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.42578125" style="4" customWidth="1"/>
-    <col min="3" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.85546875" style="4" customWidth="1"/>
     <col min="6" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" style="4" customWidth="1"/>
@@ -2104,6 +2139,9 @@
     </row>
     <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
+      <c r="C6" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
       <c r="K6" s="5"/>
@@ -2117,6 +2155,9 @@
     </row>
     <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
+      <c r="C7" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
       <c r="K7" s="5"/>
@@ -2128,14 +2169,27 @@
       <c r="AB7" s="5"/>
       <c r="AD7" s="6"/>
     </row>
-    <row r="8" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="S8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="AB8" s="5"/>
       <c r="AD8" s="6"/>
     </row>
     <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="B9" s="5"/>
+      <c r="C9" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="H9" s="5"/>
       <c r="K9" s="5"/>
@@ -2149,6 +2203,9 @@
     </row>
     <row r="10" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
+      <c r="C10" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="E10" s="5"/>
       <c r="H10" s="5"/>
       <c r="K10" s="5"/>
@@ -2162,6 +2219,9 @@
     </row>
     <row r="11" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
+      <c r="C11" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
       <c r="K11" s="5"/>
@@ -2173,20 +2233,13 @@
       <c r="AB11" s="5"/>
       <c r="AD11" s="6"/>
     </row>
-    <row r="12" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="P12" s="6"/>
-      <c r="S12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="Y12" s="5"/>
-      <c r="AB12" s="5"/>
+    <row r="12" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="AD12" s="6"/>
     </row>
     <row r="13" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="B13" s="5"/>
       <c r="E13" s="5"/>
       <c r="H13" s="5"/>
@@ -2199,13 +2252,20 @@
       <c r="AB13" s="5"/>
       <c r="AD13" s="6"/>
     </row>
-    <row r="14" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="P14" s="6"/>
+      <c r="S14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="AB14" s="5"/>
       <c r="AD14" s="6"/>
     </row>
     <row r="15" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="B15" s="5"/>
       <c r="E15" s="5"/>
       <c r="H15" s="5"/>
@@ -2244,20 +2304,13 @@
       <c r="AB17" s="5"/>
       <c r="AD17" s="6"/>
     </row>
-    <row r="18" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="P18" s="6"/>
-      <c r="S18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="Y18" s="5"/>
-      <c r="AB18" s="5"/>
+    <row r="18" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="AD18" s="6"/>
     </row>
     <row r="19" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="B19" s="5"/>
       <c r="E19" s="5"/>
       <c r="H19" s="5"/>
@@ -2270,17 +2323,21 @@
       <c r="AB19" s="5"/>
       <c r="AD19" s="6"/>
     </row>
-    <row r="20" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="P20" s="6"/>
+      <c r="S20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="AB20" s="5"/>
       <c r="AD20" s="6"/>
     </row>
     <row r="21" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="20" t="s">
-        <v>34</v>
-      </c>
       <c r="E21" s="5"/>
       <c r="H21" s="5"/>
       <c r="K21" s="5"/>
@@ -2294,9 +2351,6 @@
     </row>
     <row r="22" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
-      <c r="C22" s="20" t="s">
-        <v>35</v>
-      </c>
       <c r="E22" s="5"/>
       <c r="H22" s="5"/>
       <c r="K22" s="5"/>
@@ -2310,9 +2364,6 @@
     </row>
     <row r="23" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
-      <c r="C23" s="20" t="s">
-        <v>36</v>
-      </c>
       <c r="E23" s="5"/>
       <c r="H23" s="5"/>
       <c r="K23" s="5"/>
@@ -2324,21 +2375,17 @@
       <c r="AB23" s="5"/>
       <c r="AD23" s="6"/>
     </row>
-    <row r="24" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="P24" s="6"/>
-      <c r="S24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="Y24" s="5"/>
-      <c r="AB24" s="5"/>
+    <row r="24" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="AD24" s="6"/>
     </row>
     <row r="25" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B25" s="5"/>
+      <c r="C25" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="E25" s="5"/>
       <c r="H25" s="5"/>
       <c r="K25" s="5"/>
@@ -2350,45 +2397,31 @@
       <c r="AB25" s="5"/>
       <c r="AD25" s="6"/>
     </row>
-    <row r="26" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="5"/>
+      <c r="C26" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="P26" s="6"/>
+      <c r="S26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="AB26" s="5"/>
       <c r="AD26" s="6"/>
     </row>
     <row r="27" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="B27" s="5"/>
-      <c r="C27" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>26</v>
+      <c r="C27" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="22" t="s">
-        <v>20</v>
-      </c>
       <c r="H27" s="5"/>
-      <c r="I27" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J27" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K27" s="21"/>
-      <c r="L27" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>14</v>
-      </c>
+      <c r="K27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="22" t="s">
-        <v>17</v>
-      </c>
       <c r="P27" s="6"/>
       <c r="S27" s="5"/>
       <c r="V27" s="5"/>
@@ -2398,28 +2431,9 @@
     </row>
     <row r="28" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
-      <c r="C28" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>28</v>
-      </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="22" t="s">
-        <v>21</v>
-      </c>
       <c r="H28" s="5"/>
-      <c r="I28" s="22"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="M28" s="22" t="s">
-        <v>16</v>
-      </c>
       <c r="N28" s="5"/>
       <c r="P28" s="6"/>
       <c r="S28" s="5"/>
@@ -2441,25 +2455,45 @@
       <c r="AB29" s="5"/>
       <c r="AD29" s="6"/>
     </row>
-    <row r="30" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="P30" s="6"/>
-      <c r="S30" s="5"/>
-      <c r="V30" s="5"/>
-      <c r="Y30" s="5"/>
-      <c r="AB30" s="5"/>
+    <row r="30" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="AD30" s="6"/>
     </row>
     <row r="31" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B31" s="5"/>
+      <c r="C31" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="E31" s="5"/>
+      <c r="F31" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>20</v>
+      </c>
       <c r="H31" s="5"/>
-      <c r="K31" s="5"/>
+      <c r="I31" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K31" s="21"/>
+      <c r="L31" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="M31" s="22" t="s">
+        <v>14</v>
+      </c>
       <c r="N31" s="5"/>
+      <c r="O31" s="22" t="s">
+        <v>17</v>
+      </c>
       <c r="P31" s="6"/>
       <c r="S31" s="5"/>
       <c r="V31" s="5"/>
@@ -2467,8 +2501,79 @@
       <c r="AB31" s="5"/>
       <c r="AD31" s="6"/>
     </row>
-    <row r="32" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="C32" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="22"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="N32" s="5"/>
+      <c r="P32" s="6"/>
+      <c r="S32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="AB32" s="5"/>
       <c r="AD32" s="6"/>
+    </row>
+    <row r="33" spans="2:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="P33" s="6"/>
+      <c r="S33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="AB33" s="5"/>
+      <c r="AD33" s="6"/>
+    </row>
+    <row r="34" spans="2:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="P34" s="6"/>
+      <c r="S34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="Y34" s="5"/>
+      <c r="AB34" s="5"/>
+      <c r="AD34" s="6"/>
+    </row>
+    <row r="35" spans="2:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="P35" s="6"/>
+      <c r="S35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="AB35" s="5"/>
+      <c r="AD35" s="6"/>
+    </row>
+    <row r="36" spans="2:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AD36" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Planning update and gdd
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="233">
   <si>
     <t>Satyr</t>
   </si>
@@ -501,12 +501,6 @@
     <t>Satyr Spawn</t>
   </si>
   <si>
-    <t>Pause Manager</t>
-  </si>
-  <si>
-    <t>Main menu Manager</t>
-  </si>
-  <si>
     <t>Player respawn manager</t>
   </si>
   <si>
@@ -712,6 +706,24 @@
   </si>
   <si>
     <t>UW_ENV_STONE3</t>
+  </si>
+  <si>
+    <t>UI Manager</t>
+  </si>
+  <si>
+    <t>Level Design</t>
+  </si>
+  <si>
+    <t>Terrain</t>
+  </si>
+  <si>
+    <t>Labyrinth</t>
+  </si>
+  <si>
+    <t>Empty inventory slot</t>
+  </si>
+  <si>
+    <t>2D_HUD_INVSLOT</t>
   </si>
 </sst>
 </file>
@@ -1208,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B12:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,16 +1670,16 @@
     <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -1680,16 +1692,16 @@
     <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -1702,16 +1714,16 @@
     <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1724,16 +1736,16 @@
     <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>194</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -1746,16 +1758,16 @@
     <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="24" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -1768,16 +1780,16 @@
     <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1790,16 +1802,16 @@
     <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
@@ -1812,16 +1824,16 @@
     <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1834,16 +1846,16 @@
     <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -1856,16 +1868,16 @@
     <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="24" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -1878,16 +1890,16 @@
     <row r="32" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -2094,10 +2106,10 @@
     <row r="45" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -2112,10 +2124,10 @@
     <row r="46" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>166</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
@@ -2184,10 +2196,10 @@
     <row r="50" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
       <c r="B50" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50" s="19" t="s">
         <v>167</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>169</v>
       </c>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
@@ -2202,10 +2214,10 @@
     <row r="51" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
       <c r="B51" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" s="19" t="s">
         <v>168</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>170</v>
       </c>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
@@ -2220,10 +2232,10 @@
     <row r="52" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
       <c r="B52" s="24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
@@ -2238,10 +2250,10 @@
     <row r="53" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
       <c r="B53" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
@@ -2256,10 +2268,10 @@
     <row r="54" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="17"/>
       <c r="B54" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
@@ -2274,10 +2286,10 @@
     <row r="55" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17"/>
       <c r="B55" s="24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
@@ -2292,10 +2304,10 @@
     <row r="56" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17"/>
       <c r="B56" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
@@ -2310,10 +2322,10 @@
     <row r="57" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="B57" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
@@ -2328,10 +2340,10 @@
     <row r="58" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17"/>
       <c r="B58" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
@@ -2343,49 +2355,53 @@
       </c>
       <c r="J58" s="17"/>
     </row>
-    <row r="59" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J60" s="17"/>
-    </row>
-    <row r="61" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="17"/>
+      <c r="B59" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="15"/>
+      <c r="J59" s="17"/>
+    </row>
+    <row r="60" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J61" s="17"/>
     </row>
-    <row r="62" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J62" s="17"/>
+    </row>
+    <row r="63" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="17"/>
-    </row>
-    <row r="63" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="23" t="s">
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="17"/>
+    </row>
+    <row r="64" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="H63" s="15"/>
-      <c r="J63" s="17"/>
-    </row>
-    <row r="64" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="17"/>
-      <c r="B64" s="24" t="s">
-        <v>98</v>
-      </c>
       <c r="H64" s="15"/>
-      <c r="I64" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="J64" s="17"/>
     </row>
     <row r="65" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="17"/>
       <c r="B65" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H65" s="15"/>
       <c r="I65" s="3" t="s">
@@ -2396,58 +2412,58 @@
     <row r="66" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="17"/>
       <c r="B66" s="24" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="H66" s="15"/>
       <c r="I66" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J66" s="17"/>
+    </row>
+    <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="17"/>
+      <c r="B67" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="H67" s="15"/>
+      <c r="I67" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J66" s="17"/>
-    </row>
-    <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="23" t="s">
+      <c r="J67" s="17"/>
+    </row>
+    <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="H67" s="15"/>
-      <c r="J67" s="17"/>
-    </row>
-    <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="17"/>
-      <c r="B68" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="H68" s="15"/>
-      <c r="I68" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="J68" s="17"/>
     </row>
     <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
-      <c r="B69" s="24" t="s">
-        <v>145</v>
+      <c r="B69" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="H69" s="15"/>
       <c r="I69" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J69" s="17"/>
     </row>
     <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="17"/>
       <c r="B70" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H70" s="15"/>
       <c r="I70" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J70" s="17"/>
     </row>
     <row r="71" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="17"/>
       <c r="B71" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H71" s="15"/>
       <c r="I71" s="3" t="s">
@@ -2458,7 +2474,7 @@
     <row r="72" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="17"/>
       <c r="B72" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H72" s="15"/>
       <c r="I72" s="3" t="s">
@@ -2469,29 +2485,29 @@
     <row r="73" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="17"/>
       <c r="B73" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H73" s="15"/>
       <c r="I73" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J73" s="17"/>
     </row>
     <row r="74" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="17"/>
       <c r="B74" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H74" s="15"/>
       <c r="I74" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J74" s="17"/>
     </row>
     <row r="75" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="17"/>
       <c r="B75" s="24" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H75" s="15"/>
       <c r="I75" s="3" t="s">
@@ -2502,7 +2518,7 @@
     <row r="76" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="17"/>
       <c r="B76" s="24" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H76" s="15"/>
       <c r="I76" s="3" t="s">
@@ -2513,7 +2529,7 @@
     <row r="77" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="17"/>
       <c r="B77" s="24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H77" s="15"/>
       <c r="I77" s="3" t="s">
@@ -2524,7 +2540,7 @@
     <row r="78" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="17"/>
       <c r="B78" s="24" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H78" s="15"/>
       <c r="I78" s="3" t="s">
@@ -2532,28 +2548,28 @@
       </c>
       <c r="J78" s="17"/>
     </row>
-    <row r="79" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="23" t="s">
+    <row r="79" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="17"/>
+      <c r="B79" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="H79" s="15"/>
+      <c r="I79" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J79" s="17"/>
+    </row>
+    <row r="80" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="H79" s="15"/>
-      <c r="J79" s="17"/>
-    </row>
-    <row r="80" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="17"/>
-      <c r="B80" s="24" t="s">
-        <v>152</v>
-      </c>
       <c r="H80" s="15"/>
-      <c r="I80" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="J80" s="17"/>
     </row>
     <row r="81" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
       <c r="B81" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H81" s="15"/>
       <c r="I81" s="3" t="s">
@@ -2564,7 +2580,7 @@
     <row r="82" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="17"/>
       <c r="B82" s="24" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H82" s="15"/>
       <c r="I82" s="3" t="s">
@@ -2573,58 +2589,64 @@
       <c r="J82" s="17"/>
     </row>
     <row r="83" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="23" t="s">
+      <c r="A83" s="17"/>
+      <c r="B83" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="H83" s="15"/>
+      <c r="I83" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J83" s="17"/>
+    </row>
+    <row r="84" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H83" s="15"/>
-      <c r="J83" s="17"/>
-    </row>
-    <row r="84" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="17"/>
-      <c r="B84" s="24" t="s">
-        <v>155</v>
-      </c>
       <c r="H84" s="15"/>
-      <c r="I84" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="J84" s="17"/>
     </row>
     <row r="85" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="17"/>
       <c r="B85" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H85" s="15"/>
       <c r="I85" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J85" s="17"/>
+    </row>
+    <row r="86" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="17"/>
+      <c r="B86" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H86" s="15"/>
+      <c r="I86" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J85" s="17"/>
-    </row>
-    <row r="86" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="87" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J87" s="17"/>
-    </row>
-    <row r="88" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J86" s="17"/>
+    </row>
+    <row r="87" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J88" s="17"/>
     </row>
-    <row r="89" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J89" s="17"/>
+    </row>
+    <row r="90" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="17"/>
-    </row>
-    <row r="90" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="17"/>
-      <c r="H90" s="15"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
       <c r="J90" s="17"/>
     </row>
     <row r="91" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2637,7 +2659,12 @@
       <c r="H92" s="15"/>
       <c r="J92" s="17"/>
     </row>
-    <row r="93" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="17"/>
+      <c r="H93" s="15"/>
+      <c r="J93" s="17"/>
+    </row>
+    <row r="94" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2646,15 +2673,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD39"/>
+  <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
@@ -2765,7 +2792,13 @@
       <c r="C3" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E3" s="5"/>
+      <c r="F3" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="K3" s="5"/>
       <c r="N3" s="5"/>
@@ -2780,6 +2813,9 @@
       <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
         <v>99</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
@@ -2811,7 +2847,7 @@
     <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
@@ -2827,7 +2863,7 @@
     <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
@@ -2875,7 +2911,7 @@
     <row r="10" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E10" s="5"/>
       <c r="H10" s="5"/>
@@ -2891,7 +2927,7 @@
     <row r="11" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
@@ -2958,7 +2994,7 @@
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>122</v>
@@ -2989,10 +3025,10 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="20" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K15" s="5"/>
       <c r="N15" s="5"/>
@@ -3020,10 +3056,10 @@
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K16" s="5"/>
       <c r="N16" s="5"/>
@@ -3052,7 +3088,7 @@
         <v>121</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K17" s="5"/>
       <c r="N17" s="5"/>
@@ -3100,28 +3136,28 @@
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="20" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="J20" s="20" t="s">
         <v>157</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="20" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="20" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="P20" s="6"/>
       <c r="Q20" s="20" t="s">
@@ -3141,15 +3177,14 @@
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="20"/>
+      <c r="F21" s="20" t="s">
+        <v>156</v>
+      </c>
       <c r="G21" s="20"/>
       <c r="H21" s="5"/>
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="20" t="s">
-        <v>156</v>
-      </c>
       <c r="M21" s="20"/>
       <c r="N21" s="5"/>
       <c r="P21" s="6"/>
@@ -3159,30 +3194,49 @@
       <c r="AB21" s="5"/>
       <c r="AD21" s="6"/>
     </row>
-    <row r="22" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="5"/>
-      <c r="P22" s="6"/>
-      <c r="S22" s="5"/>
-      <c r="V22" s="5"/>
-      <c r="Y22" s="5"/>
-      <c r="AB22" s="5"/>
+    <row r="22" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="AD22" s="6"/>
     </row>
     <row r="23" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B23" s="5"/>
+      <c r="C23" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="E23" s="5"/>
+      <c r="F23" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>138</v>
+      </c>
       <c r="H23" s="5"/>
+      <c r="I23" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>203</v>
+      </c>
       <c r="K23" s="5"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
+      <c r="L23" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="M23" s="22" t="s">
+        <v>110</v>
+      </c>
       <c r="N23" s="5"/>
+      <c r="O23" s="22" t="s">
+        <v>116</v>
+      </c>
       <c r="P23" s="6"/>
+      <c r="Q23" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="S23" s="5"/>
       <c r="V23" s="5"/>
       <c r="Y23" s="5"/>
@@ -3191,61 +3245,126 @@
     </row>
     <row r="24" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
+      <c r="C24" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="E24" s="5"/>
+      <c r="F24" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="H24" s="5"/>
+      <c r="I24" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>206</v>
+      </c>
       <c r="K24" s="5"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
+      <c r="L24" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>111</v>
+      </c>
       <c r="N24" s="5"/>
+      <c r="O24" s="22" t="s">
+        <v>114</v>
+      </c>
       <c r="P24" s="6"/>
+      <c r="Q24" s="22" t="s">
+        <v>178</v>
+      </c>
       <c r="S24" s="5"/>
       <c r="V24" s="5"/>
       <c r="Y24" s="5"/>
       <c r="AB24" s="5"/>
       <c r="AD24" s="6"/>
     </row>
-    <row r="25" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+      <c r="C25" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="M25" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="N25" s="5"/>
+      <c r="O25" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="S25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="AB25" s="5"/>
       <c r="AD25" s="6"/>
     </row>
     <row r="26" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="20" t="s">
-        <v>34</v>
+      <c r="C26" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="20" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="20" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="20" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="M26" s="22" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="N26" s="5"/>
       <c r="O26" s="22" t="s">
-        <v>116</v>
+        <v>167</v>
       </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="S26" s="5"/>
       <c r="V26" s="5"/>
@@ -3255,40 +3374,40 @@
     </row>
     <row r="27" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
-      <c r="C27" s="20" t="s">
-        <v>35</v>
+      <c r="C27" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="20" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="20" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="20" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="M27" s="22" t="s">
-        <v>111</v>
+        <v>163</v>
       </c>
       <c r="N27" s="5"/>
       <c r="O27" s="22" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="22" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="S27" s="5"/>
       <c r="V27" s="5"/>
@@ -3298,40 +3417,38 @@
     </row>
     <row r="28" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
-      <c r="C28" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>56</v>
-      </c>
+      <c r="C28" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="20"/>
       <c r="E28" s="5"/>
       <c r="F28" s="20" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="20" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="20" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>112</v>
+        <v>164</v>
       </c>
       <c r="N28" s="5"/>
       <c r="O28" s="22" t="s">
-        <v>115</v>
+        <v>176</v>
       </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="22" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="S28" s="5"/>
       <c r="V28" s="5"/>
@@ -3341,40 +3458,21 @@
     </row>
     <row r="29" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
-      <c r="C29" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>61</v>
-      </c>
+      <c r="C29" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="20"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>120</v>
-      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>219</v>
-      </c>
+      <c r="J29" s="20"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="M29" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="L29" s="20"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="22" t="s">
-        <v>169</v>
-      </c>
       <c r="P29" s="6"/>
-      <c r="Q29" s="22" t="s">
-        <v>182</v>
+      <c r="Q29" s="19" t="s">
+        <v>232</v>
       </c>
       <c r="S29" s="5"/>
       <c r="V29" s="5"/>
@@ -3382,85 +3480,56 @@
       <c r="AB29" s="5"/>
       <c r="AD29" s="6"/>
     </row>
-    <row r="30" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="5"/>
-      <c r="C30" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="J30" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="K30" s="5"/>
-      <c r="L30" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="M30" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="N30" s="5"/>
-      <c r="O30" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="S30" s="5"/>
-      <c r="V30" s="5"/>
-      <c r="Y30" s="5"/>
-      <c r="AB30" s="5"/>
+    <row r="30" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="AD30" s="6"/>
     </row>
     <row r="31" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B31" s="5"/>
       <c r="C31" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="20"/>
+        <v>25</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>124</v>
+      <c r="F31" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="H31" s="5"/>
-      <c r="I31" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="J31" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="K31" s="5"/>
-      <c r="L31" s="20" t="s">
-        <v>228</v>
+      <c r="I31" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K31" s="21"/>
+      <c r="L31" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="M31" s="22" t="s">
-        <v>166</v>
+        <v>14</v>
       </c>
       <c r="N31" s="5"/>
       <c r="O31" s="22" t="s">
-        <v>178</v>
+        <v>17</v>
       </c>
       <c r="P31" s="6"/>
-      <c r="Q31" s="22" t="s">
-        <v>184</v>
+      <c r="Q31" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="R31" s="20" t="s">
+        <v>191</v>
       </c>
       <c r="S31" s="5"/>
+      <c r="T31" s="20" t="s">
+        <v>192</v>
+      </c>
       <c r="V31" s="5"/>
       <c r="Y31" s="5"/>
       <c r="AB31" s="5"/>
@@ -3468,75 +3537,93 @@
     </row>
     <row r="32" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="5"/>
-      <c r="C32" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="20"/>
+      <c r="C32" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
+      <c r="F32" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="H32" s="5"/>
-      <c r="J32" s="20"/>
+      <c r="I32" s="22"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="20"/>
+      <c r="L32" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="22" t="s">
+        <v>16</v>
+      </c>
       <c r="N32" s="5"/>
       <c r="P32" s="6"/>
+      <c r="Q32" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="R32" s="20" t="s">
+        <v>194</v>
+      </c>
       <c r="S32" s="5"/>
+      <c r="T32" s="20" t="s">
+        <v>195</v>
+      </c>
       <c r="V32" s="5"/>
       <c r="Y32" s="5"/>
       <c r="AB32" s="5"/>
       <c r="AD32" s="6"/>
     </row>
-    <row r="33" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="R33" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="S33" s="5"/>
+      <c r="T33" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="V33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="AB33" s="5"/>
       <c r="AD33" s="6"/>
     </row>
     <row r="34" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>228</v>
       </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>26</v>
+      <c r="C34" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="E34" s="5"/>
-      <c r="F34" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="22" t="s">
-        <v>20</v>
+      <c r="F34" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="H34" s="5"/>
-      <c r="I34" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J34" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K34" s="21"/>
-      <c r="L34" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="M34" s="22" t="s">
-        <v>14</v>
-      </c>
+      <c r="K34" s="5"/>
       <c r="N34" s="5"/>
-      <c r="O34" s="22" t="s">
-        <v>17</v>
-      </c>
       <c r="P34" s="6"/>
-      <c r="Q34" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="R34" s="20" t="s">
-        <v>193</v>
-      </c>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
       <c r="S34" s="5"/>
-      <c r="T34" s="20" t="s">
-        <v>194</v>
-      </c>
+      <c r="T34" s="20"/>
       <c r="V34" s="5"/>
       <c r="Y34" s="5"/>
       <c r="AB34" s="5"/>
@@ -3544,97 +3631,22 @@
     </row>
     <row r="35" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="5"/>
-      <c r="C35" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>28</v>
-      </c>
       <c r="E35" s="5"/>
-      <c r="F35" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="22" t="s">
-        <v>21</v>
-      </c>
       <c r="H35" s="5"/>
-      <c r="I35" s="22"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="M35" s="22" t="s">
-        <v>16</v>
-      </c>
       <c r="N35" s="5"/>
       <c r="P35" s="6"/>
-      <c r="Q35" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="R35" s="20" t="s">
-        <v>196</v>
-      </c>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
       <c r="S35" s="5"/>
-      <c r="T35" s="20" t="s">
-        <v>197</v>
-      </c>
+      <c r="T35" s="20"/>
       <c r="V35" s="5"/>
       <c r="Y35" s="5"/>
       <c r="AB35" s="5"/>
       <c r="AD35" s="6"/>
     </row>
-    <row r="36" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="R36" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="S36" s="5"/>
-      <c r="T36" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="V36" s="5"/>
-      <c r="Y36" s="5"/>
-      <c r="AB36" s="5"/>
+    <row r="36" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="AD36" s="6"/>
-    </row>
-    <row r="37" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="P37" s="6"/>
-      <c r="R37" s="20"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="20"/>
-      <c r="V37" s="5"/>
-      <c r="Y37" s="5"/>
-      <c r="AB37" s="5"/>
-      <c r="AD37" s="6"/>
-    </row>
-    <row r="38" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="P38" s="6"/>
-      <c r="S38" s="5"/>
-      <c r="V38" s="5"/>
-      <c r="Y38" s="5"/>
-      <c r="AB38" s="5"/>
-      <c r="AD38" s="6"/>
-    </row>
-    <row r="39" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AD39" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Dialogue manager to the planning. Finished player controller and started dialogue manager
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -459,9 +459,6 @@
     <t>Enemies</t>
   </si>
   <si>
-    <t>Game manager</t>
-  </si>
-  <si>
     <t>Quest manager</t>
   </si>
   <si>
@@ -724,6 +721,9 @@
   </si>
   <si>
     <t>2D_HUD_INVSLOT</t>
+  </si>
+  <si>
+    <t>Dialogue manager</t>
   </si>
 </sst>
 </file>
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B12:B14"/>
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,16 +1670,16 @@
     <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -1692,16 +1692,16 @@
     <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -1714,16 +1714,16 @@
     <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1736,16 +1736,16 @@
     <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -1758,16 +1758,16 @@
     <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -1780,16 +1780,16 @@
     <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1802,16 +1802,16 @@
     <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
@@ -1824,16 +1824,16 @@
     <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>215</v>
-      </c>
       <c r="E29" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1846,16 +1846,16 @@
     <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -1868,16 +1868,16 @@
     <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>219</v>
-      </c>
       <c r="E31" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -1890,16 +1890,16 @@
     <row r="32" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -2106,10 +2106,10 @@
     <row r="45" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="19" t="s">
         <v>162</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>163</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -2124,10 +2124,10 @@
     <row r="46" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
@@ -2196,10 +2196,10 @@
     <row r="50" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
       <c r="B50" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
@@ -2214,10 +2214,10 @@
     <row r="51" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
       <c r="B51" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
@@ -2232,10 +2232,10 @@
     <row r="52" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
       <c r="B52" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
@@ -2250,10 +2250,10 @@
     <row r="53" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
       <c r="B53" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
@@ -2268,10 +2268,10 @@
     <row r="54" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="17"/>
       <c r="B54" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
@@ -2286,10 +2286,10 @@
     <row r="55" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17"/>
       <c r="B55" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
@@ -2304,10 +2304,10 @@
     <row r="56" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17"/>
       <c r="B56" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
@@ -2322,10 +2322,10 @@
     <row r="57" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="B57" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
@@ -2340,10 +2340,10 @@
     <row r="58" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17"/>
       <c r="B58" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
@@ -2358,10 +2358,10 @@
     <row r="59" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="17"/>
       <c r="B59" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C59" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="C59" s="19" t="s">
-        <v>232</v>
       </c>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
@@ -2423,7 +2423,7 @@
     <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="17"/>
       <c r="B67" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="3" t="s">
@@ -2440,12 +2440,12 @@
     </row>
     <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="24" t="s">
         <v>144</v>
       </c>
       <c r="H69" s="15"/>
       <c r="I69" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J69" s="17"/>
     </row>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="H70" s="15"/>
       <c r="I70" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J70" s="17"/>
     </row>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="H73" s="15"/>
       <c r="I73" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J73" s="17"/>
     </row>
@@ -2500,14 +2500,14 @@
       </c>
       <c r="H74" s="15"/>
       <c r="I74" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J74" s="17"/>
     </row>
     <row r="75" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="17"/>
       <c r="B75" s="24" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H75" s="15"/>
       <c r="I75" s="3" t="s">
@@ -2518,7 +2518,7 @@
     <row r="76" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="17"/>
       <c r="B76" s="24" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H76" s="15"/>
       <c r="I76" s="3" t="s">
@@ -2540,7 +2540,7 @@
     <row r="78" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="17"/>
       <c r="B78" s="24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H78" s="15"/>
       <c r="I78" s="3" t="s">
@@ -2551,12 +2551,9 @@
     <row r="79" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="17"/>
       <c r="B79" s="24" t="s">
-        <v>161</v>
+        <v>232</v>
       </c>
       <c r="H79" s="15"/>
-      <c r="I79" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="J79" s="17"/>
     </row>
     <row r="80" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -2569,7 +2566,7 @@
     <row r="81" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
       <c r="B81" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H81" s="15"/>
       <c r="I81" s="3" t="s">
@@ -2580,7 +2577,7 @@
     <row r="82" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="17"/>
       <c r="B82" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H82" s="15"/>
       <c r="I82" s="3" t="s">
@@ -2591,7 +2588,7 @@
     <row r="83" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="17"/>
       <c r="B83" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H83" s="15"/>
       <c r="I83" s="3" t="s">
@@ -2609,7 +2606,7 @@
     <row r="85" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="17"/>
       <c r="B85" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H85" s="15"/>
       <c r="I85" s="3" t="s">
@@ -2620,7 +2617,7 @@
     <row r="86" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="17"/>
       <c r="B86" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H86" s="15"/>
       <c r="I86" s="3" t="s">
@@ -2676,7 +2673,7 @@
   <dimension ref="A1:AD36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,11 +2790,11 @@
         <v>98</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>98</v>
+        <v>232</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H3" s="5"/>
       <c r="K3" s="5"/>
@@ -2813,9 +2810,6 @@
       <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
@@ -2831,7 +2825,7 @@
     <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
@@ -2847,7 +2841,7 @@
     <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
@@ -2863,7 +2857,7 @@
     <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
@@ -2879,7 +2873,7 @@
     <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" s="5"/>
       <c r="H8" s="5"/>
@@ -2895,7 +2889,7 @@
     <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
       <c r="C9" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E9" s="5"/>
       <c r="H9" s="5"/>
@@ -2911,7 +2905,7 @@
     <row r="10" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E10" s="5"/>
       <c r="H10" s="5"/>
@@ -2927,7 +2921,7 @@
     <row r="11" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
@@ -2994,7 +2988,7 @@
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>122</v>
@@ -3025,10 +3019,10 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K15" s="5"/>
       <c r="N15" s="5"/>
@@ -3056,10 +3050,10 @@
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K16" s="5"/>
       <c r="N16" s="5"/>
@@ -3088,7 +3082,7 @@
         <v>121</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K17" s="5"/>
       <c r="N17" s="5"/>
@@ -3129,42 +3123,42 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P20" s="6"/>
       <c r="Q20" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R20" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S20" s="5"/>
       <c r="V20" s="5"/>
@@ -3178,7 +3172,7 @@
       <c r="D21" s="20"/>
       <c r="E21" s="5"/>
       <c r="F21" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="5"/>
@@ -3217,14 +3211,14 @@
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="J23" s="20" t="s">
         <v>202</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>203</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M23" s="22" t="s">
         <v>110</v>
@@ -3235,7 +3229,7 @@
       </c>
       <c r="P23" s="6"/>
       <c r="Q23" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S23" s="5"/>
       <c r="V23" s="5"/>
@@ -3260,14 +3254,14 @@
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="J24" s="20" t="s">
         <v>205</v>
-      </c>
-      <c r="J24" s="20" t="s">
-        <v>206</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M24" s="22" t="s">
         <v>111</v>
@@ -3278,7 +3272,7 @@
       </c>
       <c r="P24" s="6"/>
       <c r="Q24" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S24" s="5"/>
       <c r="V24" s="5"/>
@@ -3303,14 +3297,14 @@
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="J25" s="20" t="s">
         <v>208</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>209</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M25" s="22" t="s">
         <v>112</v>
@@ -3321,7 +3315,7 @@
       </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S25" s="5"/>
       <c r="V25" s="5"/>
@@ -3346,25 +3340,25 @@
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M26" s="22" t="s">
         <v>113</v>
       </c>
       <c r="N26" s="5"/>
       <c r="O26" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="S26" s="5"/>
       <c r="V26" s="5"/>
@@ -3389,25 +3383,25 @@
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="J27" s="20" t="s">
         <v>215</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>216</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M27" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N27" s="5"/>
       <c r="O27" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="S27" s="5"/>
       <c r="V27" s="5"/>
@@ -3430,25 +3424,25 @@
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="J28" s="20" t="s">
         <v>224</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>225</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N28" s="5"/>
       <c r="O28" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S28" s="5"/>
       <c r="V28" s="5"/>
@@ -3472,7 +3466,7 @@
       <c r="N29" s="5"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S29" s="5"/>
       <c r="V29" s="5"/>
@@ -3521,14 +3515,14 @@
       </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="R31" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="S31" s="5"/>
       <c r="T31" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="V31" s="5"/>
       <c r="Y31" s="5"/>
@@ -3562,14 +3556,14 @@
       <c r="N32" s="5"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="R32" s="20" t="s">
         <v>193</v>
-      </c>
-      <c r="R32" s="20" t="s">
-        <v>194</v>
       </c>
       <c r="S32" s="5"/>
       <c r="T32" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V32" s="5"/>
       <c r="Y32" s="5"/>
@@ -3584,14 +3578,14 @@
       <c r="N33" s="5"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="R33" s="20" t="s">
         <v>196</v>
-      </c>
-      <c r="R33" s="20" t="s">
-        <v>197</v>
       </c>
       <c r="S33" s="5"/>
       <c r="T33" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="V33" s="5"/>
       <c r="Y33" s="5"/>
@@ -3600,23 +3594,29 @@
     </row>
     <row r="34" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H34" s="5"/>
+      <c r="I34" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="K34" s="5"/>
       <c r="N34" s="5"/>
       <c r="P34" s="6"/>

</xml_diff>

<commit_message>
A* en shaders update (not finished yet)
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="242">
   <si>
     <t>Satyr</t>
   </si>
@@ -684,15 +684,6 @@
     <t>Sven</t>
   </si>
   <si>
-    <t>Bleeding</t>
-  </si>
-  <si>
-    <t>2D_PAR_BLEED</t>
-  </si>
-  <si>
-    <t>PAR_BLEED</t>
-  </si>
-  <si>
     <t>Minotaur breathing</t>
   </si>
   <si>
@@ -748,6 +739,18 @@
   </si>
   <si>
     <t>Dagger</t>
+  </si>
+  <si>
+    <t>Shaders</t>
+  </si>
+  <si>
+    <t>Skin shader</t>
+  </si>
+  <si>
+    <t>Makes blood appear on models</t>
+  </si>
+  <si>
+    <t>Mos shader</t>
   </si>
 </sst>
 </file>
@@ -1244,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,16 +1434,16 @@
     <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="24" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -2583,88 +2586,66 @@
       </c>
       <c r="J83" s="17"/>
     </row>
-    <row r="84" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="84" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="B84" s="12"/>
+      <c r="H84" s="15"/>
+      <c r="J84" s="17"/>
+    </row>
     <row r="85" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="17"/>
+      <c r="B85" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="H85" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="J85" s="17"/>
     </row>
-    <row r="86" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="17"/>
+      <c r="B86" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="H86" s="15"/>
       <c r="J86" s="17"/>
     </row>
-    <row r="87" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
+    <row r="87" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J88" s="17"/>
+    </row>
+    <row r="89" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J89" s="17"/>
+    </row>
+    <row r="90" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="14"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="17"/>
-    </row>
-    <row r="88" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="17"/>
-      <c r="B88" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="H88" s="15"/>
-      <c r="I88" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J88" s="17"/>
-    </row>
-    <row r="89" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="17"/>
-      <c r="B89" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="H89" s="15"/>
-      <c r="I89" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J89" s="17"/>
-    </row>
-    <row r="90" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="17"/>
-      <c r="B90" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="H90" s="15"/>
-      <c r="I90" s="3" t="s">
-        <v>75</v>
-      </c>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
       <c r="J90" s="17"/>
     </row>
     <row r="91" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="17"/>
       <c r="B91" s="24" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="H91" s="15"/>
       <c r="I91" s="3" t="s">
@@ -2675,13 +2656,13 @@
     <row r="92" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="17"/>
       <c r="B92" s="24" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="H92" s="15"/>
       <c r="I92" s="3" t="s">
@@ -2692,13 +2673,13 @@
     <row r="93" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="17"/>
       <c r="B93" s="24" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="H93" s="15"/>
       <c r="I93" s="3" t="s">
@@ -2706,7 +2687,41 @@
       </c>
       <c r="J93" s="17"/>
     </row>
-    <row r="94" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="94" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="17"/>
+      <c r="B94" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H94" s="15"/>
+      <c r="I94" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J94" s="17"/>
+    </row>
+    <row r="95" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="17"/>
+      <c r="B95" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H95" s="15"/>
+      <c r="I95" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J95" s="17"/>
+    </row>
+    <row r="96" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2717,8 +2732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2842,11 +2857,11 @@
         <v>211</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K3" s="5"/>
       <c r="N3" s="5"/>
@@ -2863,7 +2878,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
@@ -2882,7 +2897,7 @@
         <v>134</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
@@ -2901,7 +2916,7 @@
         <v>130</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
@@ -2920,7 +2935,7 @@
         <v>131</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
@@ -3027,7 +3042,7 @@
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="20" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M13" s="20" t="s">
         <v>104</v>
@@ -3130,7 +3145,7 @@
         <v>120</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="20" t="s">
@@ -3163,7 +3178,7 @@
         <v>121</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="20" t="s">

</xml_diff>

<commit_message>
Planning changes (IMPORTANT). Helm game ready. CLEANSING/EXORCISM
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="223">
   <si>
     <t>Satyr</t>
   </si>
@@ -81,45 +81,6 @@
     <t>ANIM_CHAR_SATYR</t>
   </si>
   <si>
-    <t>Theseus</t>
-  </si>
-  <si>
-    <t>UW_CHAR_THESEUS</t>
-  </si>
-  <si>
-    <t>3D_CHAR_THESEUS</t>
-  </si>
-  <si>
-    <t>RIG_CHAR_THESEUS</t>
-  </si>
-  <si>
-    <t>ANIM_CHAR_THESEUS</t>
-  </si>
-  <si>
-    <t>2D_CHAR_THESEUS</t>
-  </si>
-  <si>
-    <t>Minotaur</t>
-  </si>
-  <si>
-    <t>2D_CHAR_MINOTAUR</t>
-  </si>
-  <si>
-    <t>3D_CHAR_MINOTAUR</t>
-  </si>
-  <si>
-    <t>UW_CHAR_MINOTAUR</t>
-  </si>
-  <si>
-    <t>RIG_CHAR_MINOTAUR</t>
-  </si>
-  <si>
-    <t>ANIM_CHAR_MINOTAUR</t>
-  </si>
-  <si>
-    <t>Sunray</t>
-  </si>
-  <si>
     <t>Props</t>
   </si>
   <si>
@@ -303,12 +264,6 @@
     <t>Experience bar</t>
   </si>
   <si>
-    <t>Ability button</t>
-  </si>
-  <si>
-    <t>Ability button pressed</t>
-  </si>
-  <si>
     <t>Font</t>
   </si>
   <si>
@@ -324,15 +279,9 @@
     <t>2D_HUD_XPBAR</t>
   </si>
   <si>
-    <t>2D_HUD_ABILITYPRESS</t>
-  </si>
-  <si>
     <t>2D_HUD_FONT</t>
   </si>
   <si>
-    <t>2D_HUD_ABILITY</t>
-  </si>
-  <si>
     <t>Flower Plant</t>
   </si>
   <si>
@@ -426,9 +375,6 @@
     <t>Load manager</t>
   </si>
   <si>
-    <t>Options manager</t>
-  </si>
-  <si>
     <t>Experience manager</t>
   </si>
   <si>
@@ -540,42 +486,15 @@
     <t>3D_ENV_TORCH</t>
   </si>
   <si>
-    <t>Ruins1</t>
-  </si>
-  <si>
-    <t>Ruins2</t>
-  </si>
-  <si>
     <t>2D_ENV_RUINS1</t>
   </si>
   <si>
-    <t>Ruins3</t>
-  </si>
-  <si>
-    <t>2D_ENV_RUINS2</t>
-  </si>
-  <si>
-    <t>2D_ENV_RUINS3</t>
-  </si>
-  <si>
     <t>3D_ENV_RUINS1</t>
   </si>
   <si>
-    <t>3D_ENV_RUINS2</t>
-  </si>
-  <si>
-    <t>3D_ENV_RUINS3</t>
-  </si>
-  <si>
     <t>UW_ENV_RUINS1</t>
   </si>
   <si>
-    <t>UW_ENV_RUINS2</t>
-  </si>
-  <si>
-    <t>UW_ENV_RUINS3</t>
-  </si>
-  <si>
     <t>Tree1</t>
   </si>
   <si>
@@ -663,15 +582,9 @@
     <t>UI Manager</t>
   </si>
   <si>
-    <t>Level Design</t>
-  </si>
-  <si>
     <t>Terrain</t>
   </si>
   <si>
-    <t>Labyrinth</t>
-  </si>
-  <si>
     <t>Empty inventory slot</t>
   </si>
   <si>
@@ -681,18 +594,6 @@
     <t>Dialogue manager</t>
   </si>
   <si>
-    <t>Sven</t>
-  </si>
-  <si>
-    <t>Minotaur breathing</t>
-  </si>
-  <si>
-    <t>2D_PAR_BREATH</t>
-  </si>
-  <si>
-    <t>PAR_BREATH</t>
-  </si>
-  <si>
     <t>2D_PAR_FLIES</t>
   </si>
   <si>
@@ -751,6 +652,48 @@
   </si>
   <si>
     <t>Mos shader</t>
+  </si>
+  <si>
+    <t>Ruins modulair</t>
+  </si>
+  <si>
+    <t>4U_ENV_FLOWER</t>
+  </si>
+  <si>
+    <t>Bush1</t>
+  </si>
+  <si>
+    <t>Bush2</t>
+  </si>
+  <si>
+    <t>Bush3</t>
+  </si>
+  <si>
+    <t>2D_ENV_BUSH1</t>
+  </si>
+  <si>
+    <t>2D_ENV_BUSH2</t>
+  </si>
+  <si>
+    <t>2D_ENV_BUSH3</t>
+  </si>
+  <si>
+    <t>3D_ENV_BUSH1</t>
+  </si>
+  <si>
+    <t>3D_ENV_BUSH2</t>
+  </si>
+  <si>
+    <t>3D_ENV_BUSH3</t>
+  </si>
+  <si>
+    <t>UW_ENV_BUSH1</t>
+  </si>
+  <si>
+    <t>UW_ENV_BUSH2</t>
+  </si>
+  <si>
+    <t>UW_ENV_BUSH3</t>
   </si>
 </sst>
 </file>
@@ -902,7 +845,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -928,6 +871,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1247,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J96"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,7 +1229,7 @@
         <v>10</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
@@ -1312,693 +1256,681 @@
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="24" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="24" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="15"/>
       <c r="I5" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="15"/>
       <c r="I6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="24" t="s">
-        <v>33</v>
+        <v>204</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>203</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
+        <v>202</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>36</v>
+        <v>201</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
       <c r="I7" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="3" t="s">
-        <v>42</v>
-      </c>
+    <row r="8" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>234</v>
-      </c>
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="3" t="s">
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13"/>
+      <c r="B10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J10" s="17"/>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+      <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="24" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="15" t="s">
-        <v>57</v>
-      </c>
+      <c r="H12" s="15"/>
       <c r="I12" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="24" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
+      <c r="H13" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="I13" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="24" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="15"/>
       <c r="I14" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="24" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="H15" s="15"/>
       <c r="I15" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="24" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
       <c r="I16" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="24" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
       <c r="I17" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="J17" s="17"/>
     </row>
     <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="24" t="s">
-        <v>103</v>
+        <v>209</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>108</v>
+        <v>154</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>109</v>
+        <v>155</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="15"/>
       <c r="I18" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J18" s="17"/>
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="24" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="15"/>
       <c r="I19" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="J19" s="17"/>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="24" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
       <c r="I20" s="3" t="s">
-        <v>218</v>
+        <v>24</v>
       </c>
       <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="24" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
       <c r="I21" s="3" t="s">
-        <v>218</v>
+        <v>24</v>
       </c>
       <c r="J21" s="17"/>
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="24" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
       <c r="I22" s="3" t="s">
-        <v>218</v>
+        <v>24</v>
       </c>
       <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="24" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="15"/>
       <c r="I23" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="24" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="15"/>
       <c r="I24" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="24" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="15"/>
       <c r="I25" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="24" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="15"/>
       <c r="I26" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="24" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="15"/>
       <c r="I27" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="24" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
       <c r="I28" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="3" t="s">
-        <v>42</v>
-      </c>
+    <row r="29" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
       <c r="J30" s="17"/>
     </row>
     <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="24" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="15"/>
       <c r="I32" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="24" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
       <c r="I33" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="J33" s="17"/>
     </row>
     <row r="34" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="24" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
       <c r="I34" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="J34" s="17"/>
     </row>
-    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
-      <c r="B35" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="3" t="s">
-        <v>37</v>
-      </c>
+    <row r="35" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J35" s="17"/>
     </row>
-    <row r="36" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
       <c r="J36" s="17"/>
     </row>
     <row r="37" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="J37" s="17"/>
     </row>
     <row r="38" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="24" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -2006,17 +1938,17 @@
       <c r="G38" s="14"/>
       <c r="H38" s="15"/>
       <c r="I38" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J38" s="17"/>
     </row>
     <row r="39" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="24" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
@@ -2024,17 +1956,17 @@
       <c r="G39" s="14"/>
       <c r="H39" s="15"/>
       <c r="I39" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J39" s="17"/>
     </row>
     <row r="40" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="24" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
@@ -2042,17 +1974,17 @@
       <c r="G40" s="14"/>
       <c r="H40" s="15"/>
       <c r="I40" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J40" s="17"/>
     </row>
     <row r="41" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="24" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
@@ -2060,17 +1992,17 @@
       <c r="G41" s="14"/>
       <c r="H41" s="15"/>
       <c r="I41" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J41" s="17"/>
     </row>
     <row r="42" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="24" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
@@ -2078,17 +2010,17 @@
       <c r="G42" s="14"/>
       <c r="H42" s="15"/>
       <c r="I42" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="24" t="s">
-        <v>146</v>
+        <v>79</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
@@ -2096,17 +2028,17 @@
       <c r="G43" s="14"/>
       <c r="H43" s="15"/>
       <c r="I43" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J43" s="17"/>
     </row>
     <row r="44" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="24" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
@@ -2114,17 +2046,17 @@
       <c r="G44" s="14"/>
       <c r="H44" s="15"/>
       <c r="I44" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J44" s="17"/>
     </row>
     <row r="45" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="24" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -2132,17 +2064,17 @@
       <c r="G45" s="14"/>
       <c r="H45" s="15"/>
       <c r="I45" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J45" s="17"/>
     </row>
     <row r="46" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="24" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
@@ -2150,17 +2082,17 @@
       <c r="G46" s="14"/>
       <c r="H46" s="15"/>
       <c r="I46" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J46" s="17"/>
     </row>
     <row r="47" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="24" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
@@ -2168,17 +2100,17 @@
       <c r="G47" s="14"/>
       <c r="H47" s="15"/>
       <c r="I47" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J47" s="17"/>
     </row>
     <row r="48" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="24" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
@@ -2186,17 +2118,17 @@
       <c r="G48" s="14"/>
       <c r="H48" s="15"/>
       <c r="I48" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J48" s="17"/>
     </row>
     <row r="49" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="24" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
@@ -2204,17 +2136,17 @@
       <c r="G49" s="14"/>
       <c r="H49" s="15"/>
       <c r="I49" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J49" s="17"/>
     </row>
     <row r="50" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
       <c r="B50" s="24" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
@@ -2222,17 +2154,17 @@
       <c r="G50" s="14"/>
       <c r="H50" s="15"/>
       <c r="I50" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J50" s="17"/>
     </row>
     <row r="51" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
       <c r="B51" s="24" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
@@ -2240,17 +2172,17 @@
       <c r="G51" s="14"/>
       <c r="H51" s="15"/>
       <c r="I51" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J51" s="17"/>
     </row>
     <row r="52" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
       <c r="B52" s="24" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
@@ -2258,268 +2190,243 @@
       <c r="G52" s="14"/>
       <c r="H52" s="15"/>
       <c r="I52" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J52" s="17"/>
     </row>
     <row r="53" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
       <c r="B53" s="24" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="14"/>
       <c r="G53" s="14"/>
       <c r="H53" s="15"/>
-      <c r="I53" s="19" t="s">
-        <v>37</v>
-      </c>
       <c r="J53" s="17"/>
     </row>
-    <row r="54" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="17"/>
-      <c r="B54" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="J54" s="17"/>
-    </row>
-    <row r="55" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="17"/>
-      <c r="B55" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="19" t="s">
-        <v>37</v>
-      </c>
+    <row r="54" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J55" s="17"/>
     </row>
-    <row r="56" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="15"/>
+    <row r="56" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J56" s="17"/>
     </row>
-    <row r="57" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="17"/>
+    </row>
+    <row r="58" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H58" s="15"/>
       <c r="J58" s="17"/>
     </row>
-    <row r="59" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="17"/>
+      <c r="B59" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H59" s="15"/>
+      <c r="I59" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J59" s="17"/>
     </row>
     <row r="60" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
+      <c r="A60" s="17"/>
+      <c r="B60" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H60" s="15"/>
+      <c r="I60" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J60" s="17"/>
     </row>
-    <row r="61" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23" t="s">
-        <v>126</v>
+    <row r="61" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="17"/>
+      <c r="B61" s="24" t="s">
+        <v>117</v>
       </c>
       <c r="H61" s="15"/>
+      <c r="I61" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="J61" s="17"/>
     </row>
     <row r="62" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="17"/>
-      <c r="B62" s="24" t="s">
-        <v>83</v>
+      <c r="A62" s="23" t="s">
+        <v>110</v>
       </c>
       <c r="H62" s="15"/>
-      <c r="I62" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="J62" s="17"/>
     </row>
     <row r="63" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17"/>
       <c r="B63" s="24" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H63" s="15"/>
       <c r="I63" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="J63" s="17"/>
     </row>
     <row r="64" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="17"/>
       <c r="B64" s="24" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="H64" s="15"/>
       <c r="I64" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="J64" s="17"/>
     </row>
     <row r="65" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="23" t="s">
-        <v>127</v>
+      <c r="A65" s="17"/>
+      <c r="B65" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="H65" s="15"/>
+      <c r="I65" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J65" s="17"/>
     </row>
     <row r="66" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="17"/>
       <c r="B66" s="24" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="H66" s="15"/>
       <c r="I66" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="J66" s="17"/>
     </row>
     <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="17"/>
       <c r="B67" s="24" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="J67" s="17"/>
     </row>
     <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="17"/>
       <c r="B68" s="24" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="H68" s="15"/>
       <c r="I68" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="J68" s="17"/>
     </row>
     <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
       <c r="B69" s="24" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H69" s="15"/>
       <c r="I69" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="J69" s="17"/>
     </row>
     <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="17"/>
       <c r="B70" s="24" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H70" s="15"/>
       <c r="I70" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="J70" s="17"/>
     </row>
     <row r="71" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="17"/>
       <c r="B71" s="24" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H71" s="15"/>
       <c r="I71" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="J71" s="17"/>
     </row>
     <row r="72" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="17"/>
       <c r="B72" s="24" t="s">
-        <v>138</v>
+        <v>188</v>
       </c>
       <c r="H72" s="15"/>
-      <c r="I72" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="J72" s="17"/>
     </row>
-    <row r="73" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="17"/>
-      <c r="B73" s="24" t="s">
-        <v>142</v>
+    <row r="73" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="23" t="s">
+        <v>111</v>
       </c>
       <c r="H73" s="15"/>
-      <c r="I73" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="J73" s="17"/>
     </row>
     <row r="74" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="17"/>
       <c r="B74" s="24" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="H74" s="15"/>
       <c r="I74" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="J74" s="17"/>
     </row>
     <row r="75" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="17"/>
       <c r="B75" s="24" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="H75" s="15"/>
       <c r="I75" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="J75" s="17"/>
     </row>
     <row r="76" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="17"/>
       <c r="B76" s="24" t="s">
-        <v>217</v>
+        <v>123</v>
       </c>
       <c r="H76" s="15"/>
+      <c r="I76" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="J76" s="17"/>
     </row>
-    <row r="77" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="23" t="s">
-        <v>128</v>
+        <v>18</v>
       </c>
       <c r="H77" s="15"/>
       <c r="J77" s="17"/>
@@ -2527,201 +2434,144 @@
     <row r="78" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="17"/>
       <c r="B78" s="24" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="H78" s="15"/>
       <c r="I78" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="J78" s="17"/>
     </row>
     <row r="79" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="17"/>
       <c r="B79" s="24" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H79" s="15"/>
       <c r="I79" s="3" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="J79" s="17"/>
     </row>
     <row r="80" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="17"/>
-      <c r="B80" s="24" t="s">
-        <v>141</v>
-      </c>
+      <c r="A80" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="B80" s="12"/>
       <c r="H80" s="15"/>
-      <c r="I80" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="J80" s="17"/>
     </row>
     <row r="81" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H81" s="15"/>
+      <c r="A81" s="17"/>
+      <c r="B81" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="H81" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J81" s="17"/>
     </row>
     <row r="82" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="17"/>
       <c r="B82" s="24" t="s">
-        <v>139</v>
+        <v>208</v>
       </c>
       <c r="H82" s="15"/>
-      <c r="I82" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="J82" s="17"/>
     </row>
-    <row r="83" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="17"/>
-      <c r="B83" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="H83" s="15"/>
-      <c r="I83" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J83" s="17"/>
-    </row>
+    <row r="83" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="84" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="B84" s="12"/>
-      <c r="H84" s="15"/>
       <c r="J84" s="17"/>
     </row>
-    <row r="85" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="17"/>
-      <c r="B85" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="H85" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>75</v>
-      </c>
+    <row r="85" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J85" s="17"/>
     </row>
     <row r="86" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="17"/>
-      <c r="B86" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="H86" s="15"/>
+      <c r="A86" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
       <c r="J86" s="17"/>
     </row>
-    <row r="87" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="87" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="17"/>
+      <c r="B87" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H87" s="15"/>
+      <c r="I87" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J87" s="17"/>
+    </row>
     <row r="88" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="17"/>
+      <c r="B88" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H88" s="15"/>
+      <c r="I88" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J88" s="17"/>
     </row>
-    <row r="89" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="17"/>
+      <c r="B89" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H89" s="15"/>
+      <c r="I89" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J89" s="17"/>
     </row>
     <row r="90" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B90" s="14"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="14"/>
+      <c r="A90" s="17"/>
+      <c r="B90" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H90" s="15"/>
+      <c r="I90" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J90" s="17"/>
     </row>
-    <row r="91" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="17"/>
-      <c r="B91" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="H91" s="15"/>
-      <c r="I91" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J91" s="17"/>
-    </row>
-    <row r="92" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="17"/>
-      <c r="B92" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="H92" s="15"/>
-      <c r="I92" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J92" s="17"/>
-    </row>
-    <row r="93" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="17"/>
-      <c r="B93" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="H93" s="15"/>
-      <c r="I93" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J93" s="17"/>
-    </row>
-    <row r="94" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="17"/>
-      <c r="B94" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="H94" s="15"/>
-      <c r="I94" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J94" s="17"/>
-    </row>
-    <row r="95" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="17"/>
-      <c r="B95" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="H95" s="15"/>
-      <c r="I95" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J95" s="17"/>
-    </row>
-    <row r="96" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="91" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2730,10 +2580,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD40"/>
+  <dimension ref="A1:AD31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2753,11 +2603,11 @@
     <col min="14" max="14" width="2.85546875" style="4" customWidth="1"/>
     <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2.85546875" style="4" customWidth="1"/>
-    <col min="20" max="20" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="2.85546875" style="4" customWidth="1"/>
     <col min="23" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="2.85546875" style="4" customWidth="1"/>
@@ -2770,72 +2620,72 @@
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="5"/>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="K1" s="5"/>
       <c r="L1" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="S1" s="5"/>
       <c r="T1" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="V1" s="5"/>
       <c r="W1" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="Y1" s="5"/>
       <c r="Z1" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="AB1" s="5"/>
       <c r="AC1" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2843,27 +2693,31 @@
     </row>
     <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="1" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>239</v>
+        <v>206</v>
       </c>
       <c r="H3" s="5"/>
-      <c r="I3" s="1" t="s">
-        <v>221</v>
-      </c>
+      <c r="J3" s="20"/>
       <c r="K3" s="5"/>
+      <c r="L3" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="N3" s="5"/>
       <c r="P3" s="6"/>
       <c r="S3" s="5"/>
@@ -2875,13 +2729,14 @@
     <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="5"/>
       <c r="N4" s="5"/>
       <c r="P4" s="6"/>
@@ -2894,10 +2749,10 @@
     <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
@@ -2913,10 +2768,10 @@
     <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>229</v>
+        <v>196</v>
       </c>
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
@@ -2932,17 +2787,17 @@
     <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
       <c r="K7" s="5"/>
       <c r="N7" s="5"/>
       <c r="P7" s="6"/>
-      <c r="S7" s="5"/>
+      <c r="S7" s="17"/>
       <c r="V7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="AB7" s="5"/>
@@ -2951,7 +2806,7 @@
     <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="E8" s="5"/>
       <c r="H8" s="5"/>
@@ -2967,7 +2822,7 @@
     <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
       <c r="C9" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="E9" s="5"/>
       <c r="H9" s="5"/>
@@ -2983,7 +2838,7 @@
     <row r="10" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="E10" s="5"/>
       <c r="H10" s="5"/>
@@ -2999,7 +2854,7 @@
     <row r="11" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
@@ -3017,39 +2872,54 @@
     </row>
     <row r="13" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="20" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="20" t="s">
-        <v>117</v>
+        <v>12</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="20" t="s">
-        <v>236</v>
+        <v>100</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="N13" s="5"/>
-      <c r="P13" s="6"/>
+      <c r="O13" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="R13" s="22" t="s">
+        <v>129</v>
+      </c>
       <c r="S13" s="5"/>
+      <c r="T13" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="U13" s="20" t="s">
+        <v>178</v>
+      </c>
       <c r="V13" s="5"/>
       <c r="Y13" s="5"/>
       <c r="AB13" s="5"/>
@@ -3061,32 +2931,47 @@
         <v>13</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="20" t="s">
-        <v>118</v>
+        <v>13</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="20" t="s">
-        <v>205</v>
+        <v>101</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="N14" s="5"/>
+      <c r="O14" s="20" t="s">
+        <v>202</v>
+      </c>
       <c r="P14" s="6"/>
+      <c r="Q14" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="R14" s="22" t="s">
+        <v>130</v>
+      </c>
       <c r="S14" s="5"/>
+      <c r="T14" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="U14" s="20" t="s">
+        <v>179</v>
+      </c>
       <c r="V14" s="5"/>
       <c r="Y14" s="5"/>
       <c r="AB14" s="5"/>
@@ -3098,32 +2983,47 @@
         <v>15</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="20" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="20" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="20" t="s">
-        <v>206</v>
+        <v>102</v>
       </c>
       <c r="M15" s="20" t="s">
-        <v>168</v>
+        <v>28</v>
       </c>
       <c r="N15" s="5"/>
+      <c r="O15" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="P15" s="6"/>
+      <c r="Q15" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="R15" s="22" t="s">
+        <v>143</v>
+      </c>
       <c r="S15" s="5"/>
+      <c r="T15" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="U15" s="20" t="s">
+        <v>180</v>
+      </c>
       <c r="V15" s="5"/>
       <c r="Y15" s="5"/>
       <c r="AB15" s="5"/>
@@ -3132,31 +3032,42 @@
     <row r="16" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="20" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="5"/>
       <c r="F16" s="20" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="5"/>
       <c r="I16" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="J16" s="20" t="s">
-        <v>234</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="J16" s="20"/>
       <c r="K16" s="5"/>
       <c r="L16" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="M16" s="20" t="s">
-        <v>170</v>
+        <v>103</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>84</v>
       </c>
       <c r="N16" s="5"/>
+      <c r="O16" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="P16" s="6"/>
+      <c r="Q16" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="R16" s="22" t="s">
+        <v>144</v>
+      </c>
       <c r="S16" s="5"/>
+      <c r="T16" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="U16" s="20"/>
       <c r="V16" s="5"/>
       <c r="Y16" s="5"/>
       <c r="AB16" s="5"/>
@@ -3165,31 +3076,39 @@
     <row r="17" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
       <c r="C17" s="20" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="5"/>
       <c r="F17" s="20" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="5"/>
       <c r="I17" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>235</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="J17" s="20"/>
       <c r="K17" s="5"/>
       <c r="L17" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="M17" s="20" t="s">
-        <v>169</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="M17" s="20"/>
       <c r="N17" s="5"/>
+      <c r="O17" s="22" t="s">
+        <v>81</v>
+      </c>
       <c r="P17" s="6"/>
+      <c r="Q17" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="R17" s="22" t="s">
+        <v>145</v>
+      </c>
       <c r="S17" s="5"/>
+      <c r="T17" s="22" t="s">
+        <v>134</v>
+      </c>
       <c r="V17" s="5"/>
       <c r="Y17" s="5"/>
       <c r="AB17" s="5"/>
@@ -3198,188 +3117,195 @@
     <row r="18" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
       <c r="C18" s="20" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="5"/>
       <c r="F18" s="20" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="5"/>
       <c r="I18" s="20" t="s">
-        <v>122</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="J18" s="20"/>
       <c r="K18" s="5"/>
+      <c r="L18" s="20" t="s">
+        <v>105</v>
+      </c>
       <c r="N18" s="5"/>
+      <c r="O18" s="22" t="s">
+        <v>82</v>
+      </c>
       <c r="P18" s="6"/>
+      <c r="Q18" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="R18" s="22" t="s">
+        <v>142</v>
+      </c>
       <c r="S18" s="5"/>
+      <c r="T18" s="22" t="s">
+        <v>187</v>
+      </c>
       <c r="V18" s="5"/>
       <c r="Y18" s="5"/>
       <c r="AB18" s="5"/>
       <c r="AD18" s="6"/>
     </row>
-    <row r="19" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="20"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="P19" s="6"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="22"/>
+      <c r="V19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="AB19" s="5"/>
       <c r="AD19" s="6"/>
     </row>
-    <row r="20" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="J20" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="M20" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="N20" s="5"/>
-      <c r="O20" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="R20" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="S20" s="5"/>
-      <c r="V20" s="5"/>
-      <c r="Y20" s="5"/>
-      <c r="AB20" s="5"/>
+    <row r="20" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="AD20" s="6"/>
     </row>
     <row r="21" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="C21" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>118</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="F21" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="G21" s="20"/>
+        <v>118</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>118</v>
+      </c>
       <c r="H21" s="5"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
+      <c r="I21" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>118</v>
+      </c>
       <c r="K21" s="5"/>
-      <c r="M21" s="20"/>
+      <c r="L21" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="M21" s="20" t="s">
+        <v>122</v>
+      </c>
       <c r="N21" s="5"/>
+      <c r="O21" s="20" t="s">
+        <v>112</v>
+      </c>
       <c r="P21" s="6"/>
+      <c r="Q21" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="R21" s="20" t="s">
+        <v>123</v>
+      </c>
       <c r="S21" s="5"/>
+      <c r="T21" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="V21" s="5"/>
       <c r="Y21" s="5"/>
       <c r="AB21" s="5"/>
       <c r="AD21" s="6"/>
     </row>
-    <row r="22" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="5"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="5"/>
+      <c r="P22" s="6"/>
+      <c r="S22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="AB22" s="5"/>
       <c r="AD22" s="6"/>
     </row>
-    <row r="23" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="K23" s="5"/>
-      <c r="L23" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="M23" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="N23" s="5"/>
-      <c r="O23" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="S23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="Y23" s="5"/>
-      <c r="AB23" s="5"/>
+    <row r="23" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="AD23" s="6"/>
     </row>
     <row r="24" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B24" s="5"/>
       <c r="C24" s="20" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="20" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="20" t="s">
-        <v>189</v>
+        <v>97</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>190</v>
+        <v>106</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="M24" s="22" t="s">
-        <v>96</v>
+        <v>6</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>6</v>
       </c>
       <c r="N24" s="5"/>
-      <c r="O24" s="22" t="s">
-        <v>99</v>
+      <c r="O24" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="P24" s="6"/>
-      <c r="Q24" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="S24" s="5"/>
+      <c r="Q24" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="R24" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="S24" s="21"/>
+      <c r="T24" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="U24" s="20" t="s">
+        <v>174</v>
+      </c>
       <c r="V24" s="5"/>
       <c r="Y24" s="5"/>
       <c r="AB24" s="5"/>
@@ -3388,39 +3314,44 @@
     <row r="25" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
       <c r="C25" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="20"/>
+        <v>22</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="E25" s="5"/>
       <c r="F25" s="20" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="20" t="s">
-        <v>192</v>
+        <v>98</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>193</v>
+        <v>107</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="M25" s="22" t="s">
-        <v>97</v>
+        <v>7</v>
+      </c>
+      <c r="M25" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="N25" s="5"/>
-      <c r="O25" s="22" t="s">
-        <v>100</v>
-      </c>
       <c r="P25" s="6"/>
-      <c r="Q25" s="22" t="s">
-        <v>163</v>
+      <c r="R25" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="S25" s="5"/>
+      <c r="T25" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="U25" s="20" t="s">
+        <v>173</v>
+      </c>
       <c r="V25" s="5"/>
       <c r="Y25" s="5"/>
       <c r="AB25" s="5"/>
@@ -3428,37 +3359,43 @@
     </row>
     <row r="26" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5"/>
-      <c r="C26" s="22" t="s">
-        <v>47</v>
+      <c r="C26" s="20" t="s">
+        <v>23</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="5"/>
+      <c r="F26" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="G26" s="20" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="20" t="s">
-        <v>198</v>
+        <v>99</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>201</v>
+        <v>108</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="M26" s="22" t="s">
-        <v>98</v>
+        <v>14</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>14</v>
       </c>
       <c r="N26" s="5"/>
-      <c r="O26" s="22" t="s">
-        <v>151</v>
-      </c>
       <c r="P26" s="6"/>
-      <c r="Q26" s="22" t="s">
-        <v>164</v>
+      <c r="R26" s="20" t="s">
+        <v>92</v>
       </c>
       <c r="S26" s="5"/>
+      <c r="T26" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="U26" s="20" t="s">
+        <v>182</v>
+      </c>
       <c r="V26" s="5"/>
       <c r="Y26" s="5"/>
       <c r="AB26" s="5"/>
@@ -3467,36 +3404,33 @@
     <row r="27" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
       <c r="C27" s="22" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="5"/>
-      <c r="G27" s="20" t="s">
-        <v>108</v>
-      </c>
+      <c r="G27" s="20"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>200</v>
-      </c>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
       <c r="K27" s="5"/>
       <c r="L27" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>147</v>
+        <v>16</v>
+      </c>
+      <c r="M27" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="N27" s="5"/>
-      <c r="O27" s="22" t="s">
-        <v>152</v>
-      </c>
       <c r="P27" s="6"/>
-      <c r="Q27" s="22" t="s">
-        <v>165</v>
+      <c r="R27" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="S27" s="5"/>
+      <c r="T27" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="U27" s="20" t="s">
+        <v>175</v>
+      </c>
       <c r="V27" s="5"/>
       <c r="Y27" s="5"/>
       <c r="AB27" s="5"/>
@@ -3505,36 +3439,28 @@
     <row r="28" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
       <c r="C28" s="22" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="5"/>
-      <c r="G28" s="20" t="s">
-        <v>109</v>
-      </c>
+      <c r="G28" s="20"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>209</v>
-      </c>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="M28" s="22" t="s">
-        <v>148</v>
-      </c>
+      <c r="L28" s="20"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="22" t="s">
-        <v>160</v>
-      </c>
       <c r="P28" s="6"/>
-      <c r="Q28" s="22" t="s">
-        <v>166</v>
+      <c r="R28" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="S28" s="5"/>
+      <c r="T28" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="U28" s="20" t="s">
+        <v>176</v>
+      </c>
       <c r="V28" s="5"/>
       <c r="Y28" s="5"/>
       <c r="AB28" s="5"/>
@@ -3542,260 +3468,60 @@
     </row>
     <row r="29" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
-      <c r="C29" s="20" t="s">
-        <v>48</v>
+      <c r="C29" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="20"/>
       <c r="G29" s="20"/>
       <c r="H29" s="5"/>
+      <c r="I29" s="20"/>
       <c r="J29" s="20"/>
       <c r="K29" s="5"/>
       <c r="L29" s="20"/>
       <c r="N29" s="5"/>
       <c r="P29" s="6"/>
-      <c r="Q29" s="22" t="s">
-        <v>216</v>
+      <c r="R29" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="S29" s="5"/>
+      <c r="T29" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="U29" s="20" t="s">
+        <v>183</v>
+      </c>
       <c r="V29" s="5"/>
       <c r="Y29" s="5"/>
       <c r="AB29" s="5"/>
       <c r="AD29" s="6"/>
     </row>
-    <row r="30" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="5"/>
+      <c r="C30" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="20"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="5"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="20"/>
+      <c r="N30" s="5"/>
+      <c r="P30" s="6"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="20"/>
+      <c r="U30" s="20"/>
+      <c r="V30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="AB30" s="5"/>
       <c r="AD30" s="6"/>
     </row>
-    <row r="31" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J31" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="M31" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="N31" s="5"/>
-      <c r="O31" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P31" s="6"/>
-      <c r="S31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="Y31" s="5"/>
-      <c r="AB31" s="5"/>
+    <row r="31" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="AD31" s="6"/>
     </row>
-    <row r="32" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="5"/>
-      <c r="C32" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="22"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="M32" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="N32" s="5"/>
-      <c r="P32" s="6"/>
-      <c r="S32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="Y32" s="5"/>
-      <c r="AB32" s="5"/>
-      <c r="AD32" s="6"/>
-    </row>
-    <row r="33" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="P33" s="6"/>
-      <c r="S33" s="5"/>
-      <c r="V33" s="5"/>
-      <c r="Y33" s="5"/>
-      <c r="AB33" s="5"/>
-      <c r="AD33" s="6"/>
-    </row>
-    <row r="34" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="K34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="20"/>
-      <c r="V34" s="5"/>
-      <c r="Y34" s="5"/>
-      <c r="AB34" s="5"/>
-      <c r="AD34" s="6"/>
-    </row>
-    <row r="35" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="20"/>
-      <c r="R35" s="20"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="20"/>
-      <c r="V35" s="5"/>
-      <c r="Y35" s="5"/>
-      <c r="AB35" s="5"/>
-      <c r="AD35" s="6"/>
-    </row>
-    <row r="36" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AD36" s="6"/>
-    </row>
-    <row r="37" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="I37" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="J37" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="L37" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="M37" s="20" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="38" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="I38" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="J38" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="L38" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="M38" s="20" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="39" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C39" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="I39" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="J39" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="L39" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="M39" s="20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented scripts Water update and skybox
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1193,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,7 +2028,7 @@
       <c r="G43" s="14"/>
       <c r="H43" s="15"/>
       <c r="I43" s="19" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="J43" s="17"/>
     </row>
@@ -2582,8 +2582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD31"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2738,6 +2738,9 @@
       <c r="H4" s="5"/>
       <c r="J4" s="20"/>
       <c r="K4" s="5"/>
+      <c r="L4" s="22" t="s">
+        <v>84</v>
+      </c>
       <c r="N4" s="5"/>
       <c r="P4" s="6"/>
       <c r="S4" s="5"/>
@@ -3049,9 +3052,7 @@
       <c r="L16" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="M16" s="22" t="s">
-        <v>84</v>
-      </c>
+      <c r="M16" s="22"/>
       <c r="N16" s="5"/>
       <c r="O16" s="22" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Planning and maze. polished some scripts
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="219">
   <si>
     <t>Satyr</t>
   </si>
@@ -198,9 +198,6 @@
     <t>week 16</t>
   </si>
   <si>
-    <t xml:space="preserve">Week 17 </t>
-  </si>
-  <si>
     <t>Presentatie</t>
   </si>
   <si>
@@ -558,18 +555,6 @@
     <t>3D_ENV_STONE3</t>
   </si>
   <si>
-    <t>Spike trap</t>
-  </si>
-  <si>
-    <t>2D_ENV_SPIKETRAP</t>
-  </si>
-  <si>
-    <t>3D_ENV_SPIKETRAP</t>
-  </si>
-  <si>
-    <t>UW_ENV_SPIKETRAP</t>
-  </si>
-  <si>
     <t>UW_ENV_STONE1</t>
   </si>
   <si>
@@ -694,6 +679,9 @@
   </si>
   <si>
     <t>UW_ENV_BUSH3</t>
+  </si>
+  <si>
+    <t>Week 18</t>
   </si>
 </sst>
 </file>
@@ -1191,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:B51"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,16 +1314,16 @@
     <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="24" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -1479,16 +1467,16 @@
     <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -1501,16 +1489,16 @@
     <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -1523,16 +1511,16 @@
     <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -1545,16 +1533,16 @@
     <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="24" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -1567,16 +1555,16 @@
     <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -1589,16 +1577,16 @@
     <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
@@ -1611,16 +1599,16 @@
     <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -1633,16 +1621,16 @@
     <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="E22" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -1655,16 +1643,16 @@
     <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -1677,16 +1665,16 @@
     <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1699,16 +1687,16 @@
     <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="24" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -1721,16 +1709,16 @@
     <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="24" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -1743,16 +1731,16 @@
     <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="24" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1762,43 +1750,43 @@
       </c>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="3" t="s">
-        <v>29</v>
-      </c>
+    <row r="28" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
       <c r="J29" s="17"/>
     </row>
     <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="J30" s="17"/>
     </row>
     <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1807,19 +1795,19 @@
         <v>93</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="15"/>
       <c r="I31" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="J31" s="17"/>
     </row>
@@ -1829,13 +1817,13 @@
         <v>94</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -1851,59 +1839,55 @@
         <v>95</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
       <c r="I33" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J33" s="17"/>
     </row>
-    <row r="34" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="3" t="s">
-        <v>24</v>
-      </c>
+    <row r="34" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J34" s="17"/>
     </row>
-    <row r="35" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
       <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="17"/>
+      <c r="B36" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="C36" s="19" t="s">
+        <v>79</v>
+      </c>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="J36" s="17"/>
     </row>
     <row r="37" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -1963,10 +1947,10 @@
     <row r="40" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="24" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
@@ -1981,7 +1965,7 @@
     <row r="41" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>129</v>
@@ -1999,10 +1983,10 @@
     <row r="42" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="24" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
@@ -2010,17 +1994,17 @@
       <c r="G42" s="14"/>
       <c r="H42" s="15"/>
       <c r="I42" s="19" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="24" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>84</v>
+        <v>132</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
@@ -2028,7 +2012,7 @@
       <c r="G43" s="14"/>
       <c r="H43" s="15"/>
       <c r="I43" s="19" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="J43" s="17"/>
     </row>
@@ -2053,10 +2037,10 @@
     <row r="45" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="24" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -2179,62 +2163,55 @@
     <row r="52" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
       <c r="B52" s="24" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="14"/>
       <c r="G52" s="14"/>
       <c r="H52" s="15"/>
-      <c r="I52" s="19" t="s">
-        <v>29</v>
-      </c>
       <c r="J52" s="17"/>
     </row>
-    <row r="53" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="17"/>
-      <c r="B53" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="15"/>
-      <c r="J53" s="17"/>
-    </row>
-    <row r="54" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J54" s="17"/>
+    </row>
+    <row r="55" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J55" s="17"/>
     </row>
-    <row r="56" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
       <c r="J56" s="17"/>
     </row>
-    <row r="57" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
+    <row r="57" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="H57" s="15"/>
       <c r="J57" s="17"/>
     </row>
-    <row r="58" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="23" t="s">
-        <v>109</v>
+    <row r="58" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="17"/>
+      <c r="B58" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="H58" s="15"/>
+      <c r="I58" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J58" s="17"/>
     </row>
     <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2244,14 +2221,14 @@
       </c>
       <c r="H59" s="15"/>
       <c r="I59" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J59" s="17"/>
     </row>
     <row r="60" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17"/>
       <c r="B60" s="24" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="H60" s="15"/>
       <c r="I60" s="3" t="s">
@@ -2260,21 +2237,21 @@
       <c r="J60" s="17"/>
     </row>
     <row r="61" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="17"/>
-      <c r="B61" s="24" t="s">
-        <v>117</v>
+      <c r="A61" s="23" t="s">
+        <v>109</v>
       </c>
       <c r="H61" s="15"/>
-      <c r="I61" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="J61" s="17"/>
     </row>
     <row r="62" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="23" t="s">
-        <v>110</v>
+      <c r="A62" s="17"/>
+      <c r="B62" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="H62" s="15"/>
+      <c r="I62" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J62" s="17"/>
     </row>
     <row r="63" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2284,7 +2261,7 @@
       </c>
       <c r="H63" s="15"/>
       <c r="I63" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J63" s="17"/>
     </row>
@@ -2295,7 +2272,7 @@
       </c>
       <c r="H64" s="15"/>
       <c r="I64" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J64" s="17"/>
     </row>
@@ -2306,7 +2283,7 @@
       </c>
       <c r="H65" s="15"/>
       <c r="I65" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J65" s="17"/>
     </row>
@@ -2317,29 +2294,29 @@
       </c>
       <c r="H66" s="15"/>
       <c r="I66" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J66" s="17"/>
     </row>
     <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="17"/>
       <c r="B67" s="24" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J67" s="17"/>
     </row>
     <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="17"/>
       <c r="B68" s="24" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H68" s="15"/>
       <c r="I68" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J68" s="17"/>
     </row>
@@ -2350,45 +2327,45 @@
       </c>
       <c r="H69" s="15"/>
       <c r="I69" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J69" s="17"/>
     </row>
     <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="17"/>
       <c r="B70" s="24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H70" s="15"/>
       <c r="I70" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J70" s="17"/>
     </row>
     <row r="71" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="17"/>
       <c r="B71" s="24" t="s">
-        <v>127</v>
+        <v>183</v>
       </c>
       <c r="H71" s="15"/>
-      <c r="I71" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="J71" s="17"/>
     </row>
-    <row r="72" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="17"/>
-      <c r="B72" s="24" t="s">
-        <v>188</v>
+    <row r="72" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="23" t="s">
+        <v>110</v>
       </c>
       <c r="H72" s="15"/>
       <c r="J72" s="17"/>
     </row>
-    <row r="73" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="23" t="s">
-        <v>111</v>
+    <row r="73" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="17"/>
+      <c r="B73" s="24" t="s">
+        <v>117</v>
       </c>
       <c r="H73" s="15"/>
+      <c r="I73" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J73" s="17"/>
     </row>
     <row r="74" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2398,37 +2375,37 @@
       </c>
       <c r="H74" s="15"/>
       <c r="I74" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J74" s="17"/>
     </row>
     <row r="75" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="17"/>
       <c r="B75" s="24" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H75" s="15"/>
       <c r="I75" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J75" s="17"/>
     </row>
     <row r="76" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="17"/>
-      <c r="B76" s="24" t="s">
-        <v>123</v>
+      <c r="A76" s="23" t="s">
+        <v>18</v>
       </c>
       <c r="H76" s="15"/>
-      <c r="I76" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="J76" s="17"/>
     </row>
     <row r="77" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="23" t="s">
-        <v>18</v>
+      <c r="A77" s="17"/>
+      <c r="B77" s="24" t="s">
+        <v>120</v>
       </c>
       <c r="H77" s="15"/>
+      <c r="I77" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J77" s="17"/>
     </row>
     <row r="78" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2443,135 +2420,124 @@
       <c r="J78" s="17"/>
     </row>
     <row r="79" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="17"/>
-      <c r="B79" s="24" t="s">
-        <v>122</v>
-      </c>
+      <c r="A79" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B79" s="12"/>
       <c r="H79" s="15"/>
-      <c r="I79" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="J79" s="17"/>
     </row>
     <row r="80" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="B80" s="12"/>
-      <c r="H80" s="15"/>
+      <c r="A80" s="17"/>
+      <c r="B80" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="H80" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J80" s="17"/>
     </row>
     <row r="81" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
       <c r="B81" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="H81" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="I81" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="H81" s="15"/>
       <c r="J81" s="17"/>
     </row>
-    <row r="82" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="17"/>
-      <c r="B82" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="H82" s="15"/>
-      <c r="J82" s="17"/>
-    </row>
-    <row r="83" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="84" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="83" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J83" s="17"/>
+    </row>
+    <row r="84" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J84" s="17"/>
     </row>
-    <row r="85" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
       <c r="J85" s="17"/>
     </row>
     <row r="86" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
+      <c r="A86" s="17"/>
+      <c r="B86" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H86" s="15"/>
+      <c r="I86" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J86" s="17"/>
     </row>
     <row r="87" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="17"/>
       <c r="B87" s="24" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H87" s="15"/>
       <c r="I87" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J87" s="17"/>
     </row>
     <row r="88" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="17"/>
       <c r="B88" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="H88" s="15"/>
       <c r="I88" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J88" s="17"/>
     </row>
     <row r="89" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="17"/>
       <c r="B89" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="H89" s="15"/>
       <c r="I89" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J89" s="17"/>
     </row>
-    <row r="90" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="17"/>
-      <c r="B90" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="H90" s="15"/>
-      <c r="I90" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J90" s="17"/>
-    </row>
-    <row r="91" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="90" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2582,8 +2548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2647,45 +2613,45 @@
         <v>56</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O1" s="5"/>
       <c r="P1" s="1" t="s">
-        <v>57</v>
+        <v>218</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S1" s="5"/>
       <c r="T1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V1" s="5"/>
       <c r="W1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="Y1" s="5"/>
       <c r="Z1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="AB1" s="5"/>
       <c r="AC1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2694,30 +2660,30 @@
     </row>
     <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H3" s="5"/>
       <c r="J3" s="20"/>
       <c r="K3" s="5"/>
       <c r="L3" s="20" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="5"/>
@@ -2730,17 +2696,17 @@
     <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
       <c r="J4" s="20"/>
       <c r="K4" s="5"/>
       <c r="L4" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="5"/>
@@ -2753,10 +2719,10 @@
     <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
@@ -2772,10 +2738,10 @@
     <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
@@ -2791,10 +2757,10 @@
     <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
@@ -2810,7 +2776,7 @@
     <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E8" s="5"/>
       <c r="H8" s="5"/>
@@ -2826,7 +2792,7 @@
     <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
       <c r="C9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E9" s="5"/>
       <c r="H9" s="5"/>
@@ -2842,7 +2808,7 @@
     <row r="10" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E10" s="5"/>
       <c r="H10" s="5"/>
@@ -2858,7 +2824,7 @@
     <row r="11" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
@@ -2902,7 +2868,7 @@
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M13" s="20" t="s">
         <v>26</v>
@@ -2910,21 +2876,19 @@
       <c r="N13" s="25"/>
       <c r="O13" s="5"/>
       <c r="P13" s="20" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="Q13" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R13" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S13" s="5"/>
       <c r="T13" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="U13" s="20" t="s">
-        <v>178</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="U13" s="20"/>
       <c r="V13" s="5"/>
       <c r="Y13" s="5"/>
       <c r="AB13" s="5"/>
@@ -2954,7 +2918,7 @@
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M14" s="20" t="s">
         <v>27</v>
@@ -2962,21 +2926,19 @@
       <c r="N14" s="25"/>
       <c r="O14" s="5"/>
       <c r="P14" s="20" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="Q14" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R14" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S14" s="5"/>
       <c r="T14" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="U14" s="20" t="s">
-        <v>179</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="U14" s="20"/>
       <c r="V14" s="5"/>
       <c r="Y14" s="5"/>
       <c r="AB14" s="5"/>
@@ -3006,7 +2968,7 @@
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M15" s="20" t="s">
         <v>28</v>
@@ -3014,21 +2976,19 @@
       <c r="N15" s="25"/>
       <c r="O15" s="5"/>
       <c r="P15" s="20" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="Q15" s="20" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="R15" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S15" s="5"/>
       <c r="T15" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="U15" s="20" t="s">
-        <v>180</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="U15" s="20"/>
       <c r="V15" s="5"/>
       <c r="Y15" s="5"/>
       <c r="AB15" s="5"/>
@@ -3052,23 +3012,23 @@
       <c r="J16" s="20"/>
       <c r="K16" s="5"/>
       <c r="L16" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M16" s="22"/>
       <c r="N16" s="25"/>
       <c r="O16" s="5"/>
       <c r="P16" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q16" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R16" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S16" s="5"/>
       <c r="T16" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="U16" s="20"/>
       <c r="V16" s="5"/>
@@ -3094,23 +3054,23 @@
       <c r="J17" s="20"/>
       <c r="K17" s="5"/>
       <c r="L17" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M17" s="20"/>
       <c r="N17" s="25"/>
       <c r="O17" s="5"/>
       <c r="P17" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q17" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R17" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="S17" s="5"/>
       <c r="T17" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V17" s="5"/>
       <c r="Y17" s="5"/>
@@ -3135,22 +3095,22 @@
       <c r="J18" s="20"/>
       <c r="K18" s="5"/>
       <c r="L18" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="5"/>
       <c r="P18" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q18" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R18" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S18" s="5"/>
       <c r="T18" s="22" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="V18" s="5"/>
       <c r="Y18" s="5"/>
@@ -3172,7 +3132,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="5"/>
       <c r="P19" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S19" s="5"/>
       <c r="T19" s="22"/>
@@ -3187,50 +3147,50 @@
     </row>
     <row r="21" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N21" s="25"/>
       <c r="O21" s="5"/>
       <c r="P21" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q21" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R21" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S21" s="5"/>
       <c r="T21" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V21" s="5"/>
       <c r="Y21" s="5"/>
@@ -3274,17 +3234,17 @@
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="20" t="s">
@@ -3296,20 +3256,20 @@
       <c r="N24" s="25"/>
       <c r="O24" s="5"/>
       <c r="P24" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="R24" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S24" s="21"/>
       <c r="T24" s="20" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="U24" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V24" s="5"/>
       <c r="Y24" s="5"/>
@@ -3326,17 +3286,17 @@
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="20" t="s">
@@ -3348,14 +3308,14 @@
       <c r="N25" s="25"/>
       <c r="O25" s="5"/>
       <c r="R25" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S25" s="5"/>
       <c r="T25" s="20" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="U25" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="V25" s="5"/>
       <c r="Y25" s="5"/>
@@ -3370,17 +3330,17 @@
       <c r="D26" s="20"/>
       <c r="E26" s="5"/>
       <c r="F26" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="20" t="s">
@@ -3392,14 +3352,14 @@
       <c r="N26" s="25"/>
       <c r="O26" s="5"/>
       <c r="R26" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S26" s="5"/>
       <c r="T26" s="20" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="U26" s="20" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="V26" s="5"/>
       <c r="Y26" s="5"/>
@@ -3427,14 +3387,14 @@
       <c r="N27" s="25"/>
       <c r="O27" s="5"/>
       <c r="R27" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S27" s="5"/>
       <c r="T27" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="U27" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="V27" s="5"/>
       <c r="Y27" s="5"/>
@@ -3457,14 +3417,14 @@
       <c r="N28" s="6"/>
       <c r="O28" s="5"/>
       <c r="R28" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S28" s="5"/>
       <c r="T28" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U28" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="V28" s="5"/>
       <c r="Y28" s="5"/>
@@ -3487,14 +3447,14 @@
       <c r="N29" s="6"/>
       <c r="O29" s="5"/>
       <c r="R29" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S29" s="5"/>
       <c r="T29" s="20" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="U29" s="20" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="V29" s="5"/>
       <c r="Y29" s="5"/>

</xml_diff>

<commit_message>
planning update & game update
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="219">
   <si>
     <t>Satyr</t>
   </si>
@@ -1181,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,7 +1329,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
       <c r="I7" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J7" s="17"/>
     </row>
@@ -2548,8 +2548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,8 +2875,8 @@
       </c>
       <c r="N13" s="25"/>
       <c r="O13" s="5"/>
-      <c r="P13" s="20" t="s">
-        <v>198</v>
+      <c r="P13" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="Q13" s="20" t="s">
         <v>86</v>
@@ -2925,8 +2925,8 @@
       </c>
       <c r="N14" s="25"/>
       <c r="O14" s="5"/>
-      <c r="P14" s="20" t="s">
-        <v>197</v>
+      <c r="P14" s="22" t="s">
+        <v>79</v>
       </c>
       <c r="Q14" s="20" t="s">
         <v>88</v>
@@ -2975,8 +2975,8 @@
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="20" t="s">
-        <v>196</v>
+      <c r="P15" s="22" t="s">
+        <v>80</v>
       </c>
       <c r="Q15" s="20" t="s">
         <v>205</v>
@@ -3011,14 +3011,11 @@
       </c>
       <c r="J16" s="20"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="20" t="s">
-        <v>102</v>
-      </c>
       <c r="M16" s="22"/>
       <c r="N16" s="25"/>
       <c r="O16" s="5"/>
       <c r="P16" s="22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q16" s="20" t="s">
         <v>149</v>
@@ -3053,14 +3050,11 @@
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="20" t="s">
-        <v>103</v>
-      </c>
       <c r="M17" s="20"/>
       <c r="N17" s="25"/>
       <c r="O17" s="5"/>
       <c r="P17" s="22" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="Q17" s="20" t="s">
         <v>151</v>
@@ -3094,14 +3088,8 @@
       </c>
       <c r="J18" s="20"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="20" t="s">
-        <v>104</v>
-      </c>
       <c r="N18" s="6"/>
       <c r="O18" s="5"/>
-      <c r="P18" s="22" t="s">
-        <v>81</v>
-      </c>
       <c r="Q18" s="20" t="s">
         <v>150</v>
       </c>
@@ -3131,9 +3119,6 @@
       <c r="L19" s="20"/>
       <c r="N19" s="6"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="22" t="s">
-        <v>82</v>
-      </c>
       <c r="S19" s="5"/>
       <c r="T19" s="22"/>
       <c r="V19" s="5"/>
@@ -3255,11 +3240,11 @@
       </c>
       <c r="N24" s="25"/>
       <c r="O24" s="5"/>
-      <c r="P24" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>204</v>
+      <c r="P24" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q24" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="R24" s="20" t="s">
         <v>87</v>
@@ -3307,6 +3292,12 @@
       </c>
       <c r="N25" s="25"/>
       <c r="O25" s="5"/>
+      <c r="P25" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q25" s="20" t="s">
+        <v>103</v>
+      </c>
       <c r="R25" s="20" t="s">
         <v>90</v>
       </c>
@@ -3351,6 +3342,12 @@
       </c>
       <c r="N26" s="25"/>
       <c r="O26" s="5"/>
+      <c r="P26" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q26" s="20" t="s">
+        <v>104</v>
+      </c>
       <c r="R26" s="20" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Planning update & Scene update
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliek\OneDrive\Documenten\GameLab2\Documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliek\OneDrive\Documenten\GameLab_2\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="198">
   <si>
     <t>Satyr</t>
   </si>
@@ -492,78 +492,24 @@
     <t>UW_ENV_RUINS1</t>
   </si>
   <si>
-    <t>Tree1</t>
-  </si>
-  <si>
-    <t>Tree2</t>
-  </si>
-  <si>
-    <t>Tree3</t>
-  </si>
-  <si>
     <t>2D_ENV_TREE1</t>
   </si>
   <si>
-    <t>2D_ENV_TREE2</t>
-  </si>
-  <si>
-    <t>2D_ENV_TREE3</t>
-  </si>
-  <si>
     <t>3D_ENV_TREE1</t>
   </si>
   <si>
-    <t>3D_ENV_TREE2</t>
-  </si>
-  <si>
-    <t>3D_ENV_TREE3</t>
-  </si>
-  <si>
     <t>UW_ENV_TREE1</t>
   </si>
   <si>
-    <t>UW_ENV_TREE2</t>
-  </si>
-  <si>
-    <t>UW_ENV_TREE3</t>
-  </si>
-  <si>
-    <t>Stone1</t>
-  </si>
-  <si>
-    <t>Stone2</t>
-  </si>
-  <si>
-    <t>Stone3</t>
-  </si>
-  <si>
     <t>2D_ENV_STONE1</t>
   </si>
   <si>
     <t>3D_ENV_STONE1</t>
   </si>
   <si>
-    <t>3D_ENV_STONE2</t>
-  </si>
-  <si>
-    <t>2D_ENV_STONE2</t>
-  </si>
-  <si>
-    <t>2D_ENV_STONE3</t>
-  </si>
-  <si>
-    <t>3D_ENV_STONE3</t>
-  </si>
-  <si>
     <t>UW_ENV_STONE1</t>
   </si>
   <si>
-    <t>UW_ENV_STONE2</t>
-  </si>
-  <si>
-    <t>UW_ENV_STONE3</t>
-  </si>
-  <si>
     <t>UI Manager</t>
   </si>
   <si>
@@ -645,43 +591,34 @@
     <t>4U_ENV_FLOWER</t>
   </si>
   <si>
-    <t>Bush1</t>
-  </si>
-  <si>
-    <t>Bush2</t>
-  </si>
-  <si>
-    <t>Bush3</t>
-  </si>
-  <si>
     <t>2D_ENV_BUSH1</t>
   </si>
   <si>
-    <t>2D_ENV_BUSH2</t>
-  </si>
-  <si>
-    <t>2D_ENV_BUSH3</t>
-  </si>
-  <si>
     <t>3D_ENV_BUSH1</t>
   </si>
   <si>
-    <t>3D_ENV_BUSH2</t>
-  </si>
-  <si>
-    <t>3D_ENV_BUSH3</t>
-  </si>
-  <si>
     <t>UW_ENV_BUSH1</t>
   </si>
   <si>
-    <t>UW_ENV_BUSH2</t>
-  </si>
-  <si>
-    <t>UW_ENV_BUSH3</t>
-  </si>
-  <si>
     <t>Week 18</t>
+  </si>
+  <si>
+    <t>Hadewij</t>
+  </si>
+  <si>
+    <t>Nathaly</t>
+  </si>
+  <si>
+    <t>Tree's</t>
+  </si>
+  <si>
+    <t>Bushes</t>
+  </si>
+  <si>
+    <t>Stone's</t>
+  </si>
+  <si>
+    <t>Satyr Animaties</t>
   </si>
 </sst>
 </file>
@@ -703,7 +640,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -794,6 +731,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -833,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -860,6 +803,8 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1179,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,16 +1259,16 @@
     <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="24" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -1504,7 +1449,7 @@
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
       <c r="I16" s="3" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="J16" s="17"/>
     </row>
@@ -1533,7 +1478,7 @@
     <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="24" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>152</v>
@@ -1555,126 +1500,99 @@
     <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="15"/>
       <c r="I19" s="3" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="J19" s="17"/>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="24" t="s">
-        <v>156</v>
+        <v>196</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="E20" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
       <c r="I20" s="3" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="24" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
       <c r="I21" s="3" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="J21" s="17"/>
     </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="3" t="s">
-        <v>24</v>
-      </c>
+    <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>177</v>
-      </c>
+      <c r="A23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
       <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="24" t="s">
-        <v>169</v>
+        <v>92</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>174</v>
+        <v>96</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>175</v>
+        <v>97</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>178</v>
+        <v>98</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1687,60 +1605,60 @@
     <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="24" t="s">
-        <v>206</v>
+        <v>93</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>209</v>
+        <v>99</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>212</v>
+        <v>100</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>215</v>
+        <v>101</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="15"/>
       <c r="I25" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="24" t="s">
-        <v>207</v>
+        <v>94</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>210</v>
+        <v>102</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>213</v>
+        <v>103</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>216</v>
+        <v>104</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="15"/>
       <c r="I26" s="3" t="s">
-        <v>24</v>
+        <v>193</v>
       </c>
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="24" t="s">
-        <v>208</v>
+        <v>95</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>211</v>
+        <v>105</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>214</v>
+        <v>106</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>217</v>
+        <v>107</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1753,9 +1671,9 @@
     <row r="28" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>18</v>
+    <row r="29" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -1767,118 +1685,121 @@
       <c r="I29" s="14"/>
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
+    <row r="30" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="17"/>
       <c r="B30" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>98</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="15"/>
-      <c r="I30" s="3" t="s">
-        <v>24</v>
+      <c r="I30" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
+    <row r="31" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="17"/>
       <c r="B31" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>101</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="15"/>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="19" t="s">
         <v>29</v>
       </c>
       <c r="J31" s="17"/>
     </row>
-    <row r="32" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
+    <row r="32" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="17"/>
       <c r="B32" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>104</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="15"/>
-      <c r="I32" s="3" t="s">
+      <c r="I32" s="19" t="s">
         <v>29</v>
       </c>
       <c r="J32" s="17"/>
     </row>
-    <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
+    <row r="33" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="17"/>
       <c r="B33" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>107</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
-      <c r="I33" s="3" t="s">
-        <v>24</v>
+      <c r="I33" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="J33" s="17"/>
     </row>
-    <row r="34" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="17"/>
+      <c r="B34" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="J34" s="17"/>
     </row>
     <row r="35" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="24" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
@@ -1886,17 +1807,17 @@
       <c r="G36" s="14"/>
       <c r="H36" s="15"/>
       <c r="I36" s="19" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="J36" s="17"/>
     </row>
     <row r="37" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="24" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
@@ -1911,10 +1832,10 @@
     <row r="38" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="24" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -1929,10 +1850,10 @@
     <row r="39" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="24" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
@@ -1947,10 +1868,10 @@
     <row r="40" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="24" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
@@ -1965,10 +1886,10 @@
     <row r="41" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="24" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
@@ -1983,10 +1904,10 @@
     <row r="42" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="24" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
@@ -1994,17 +1915,17 @@
       <c r="G42" s="14"/>
       <c r="H42" s="15"/>
       <c r="I42" s="19" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="24" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
@@ -2019,10 +1940,10 @@
     <row r="44" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="24" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
@@ -2037,10 +1958,10 @@
     <row r="45" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="24" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -2055,158 +1976,112 @@
     <row r="46" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="24" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="G46" s="14"/>
       <c r="H46" s="15"/>
-      <c r="I46" s="19" t="s">
-        <v>29</v>
-      </c>
       <c r="J46" s="17"/>
     </row>
-    <row r="47" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
-      <c r="B47" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="J47" s="17"/>
-    </row>
-    <row r="48" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
-      <c r="B48" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="19" t="s">
-        <v>29</v>
-      </c>
+    <row r="47" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J48" s="17"/>
     </row>
-    <row r="49" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="17"/>
-      <c r="B49" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="19" t="s">
-        <v>29</v>
-      </c>
+    <row r="49" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J49" s="17"/>
     </row>
-    <row r="50" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>146</v>
-      </c>
+    <row r="50" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
       <c r="J50" s="17"/>
     </row>
     <row r="51" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="17"/>
-      <c r="B51" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
+      <c r="A51" s="23" t="s">
+        <v>108</v>
+      </c>
       <c r="H51" s="15"/>
-      <c r="I51" s="19" t="s">
-        <v>29</v>
-      </c>
       <c r="J51" s="17"/>
     </row>
-    <row r="52" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
       <c r="B52" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
+        <v>69</v>
+      </c>
       <c r="H52" s="15"/>
+      <c r="I52" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J52" s="17"/>
     </row>
-    <row r="53" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="17"/>
+      <c r="B53" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H53" s="15"/>
+      <c r="I53" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J53" s="17"/>
+    </row>
     <row r="54" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="17"/>
+      <c r="B54" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="H54" s="15"/>
+      <c r="I54" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J54" s="17"/>
     </row>
-    <row r="55" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H55" s="15"/>
       <c r="J55" s="17"/>
     </row>
     <row r="56" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="H56" s="15"/>
+      <c r="I56" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J56" s="17"/>
     </row>
-    <row r="57" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="23" t="s">
-        <v>108</v>
+    <row r="57" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="17"/>
+      <c r="B57" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="H57" s="15"/>
+      <c r="I57" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J57" s="17"/>
     </row>
     <row r="58" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17"/>
       <c r="B58" s="24" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="H58" s="15"/>
       <c r="I58" s="3" t="s">
@@ -2217,7 +2092,7 @@
     <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="17"/>
       <c r="B59" s="24" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="H59" s="15"/>
       <c r="I59" s="3" t="s">
@@ -2228,36 +2103,40 @@
     <row r="60" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17"/>
       <c r="B60" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H60" s="15"/>
       <c r="I60" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J60" s="17"/>
     </row>
     <row r="61" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23" t="s">
-        <v>109</v>
+      <c r="A61" s="17"/>
+      <c r="B61" s="24" t="s">
+        <v>119</v>
       </c>
       <c r="H61" s="15"/>
+      <c r="I61" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J61" s="17"/>
     </row>
     <row r="62" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="17"/>
       <c r="B62" s="24" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="H62" s="15"/>
       <c r="I62" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J62" s="17"/>
     </row>
     <row r="63" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17"/>
       <c r="B63" s="24" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="H63" s="15"/>
       <c r="I63" s="3" t="s">
@@ -2268,7 +2147,7 @@
     <row r="64" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="17"/>
       <c r="B64" s="24" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="H64" s="15"/>
       <c r="I64" s="3" t="s">
@@ -2279,162 +2158,142 @@
     <row r="65" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="17"/>
       <c r="B65" s="24" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="H65" s="15"/>
-      <c r="I65" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="J65" s="17"/>
     </row>
-    <row r="66" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="17"/>
-      <c r="B66" s="24" t="s">
-        <v>115</v>
+    <row r="66" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="23" t="s">
+        <v>110</v>
       </c>
       <c r="H66" s="15"/>
-      <c r="I66" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="J66" s="17"/>
     </row>
     <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="17"/>
       <c r="B67" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J67" s="17"/>
     </row>
     <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="17"/>
       <c r="B68" s="24" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H68" s="15"/>
       <c r="I68" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J68" s="17"/>
     </row>
     <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
       <c r="B69" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H69" s="15"/>
       <c r="I69" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J69" s="17"/>
     </row>
     <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="17"/>
-      <c r="B70" s="24" t="s">
-        <v>126</v>
+      <c r="A70" s="23" t="s">
+        <v>18</v>
       </c>
       <c r="H70" s="15"/>
-      <c r="I70" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="J70" s="17"/>
     </row>
     <row r="71" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="17"/>
       <c r="B71" s="24" t="s">
-        <v>183</v>
+        <v>120</v>
       </c>
       <c r="H71" s="15"/>
+      <c r="I71" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J71" s="17"/>
     </row>
-    <row r="72" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="23" t="s">
-        <v>110</v>
+    <row r="72" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="17"/>
+      <c r="B72" s="24" t="s">
+        <v>121</v>
       </c>
       <c r="H72" s="15"/>
+      <c r="I72" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J72" s="17"/>
     </row>
     <row r="73" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="17"/>
-      <c r="B73" s="24" t="s">
-        <v>117</v>
-      </c>
+      <c r="A73" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B73" s="12"/>
       <c r="H73" s="15"/>
-      <c r="I73" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="J73" s="17"/>
     </row>
     <row r="74" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="17"/>
       <c r="B74" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="H74" s="15"/>
+        <v>183</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>184</v>
+      </c>
       <c r="I74" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J74" s="17"/>
     </row>
     <row r="75" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="17"/>
       <c r="B75" s="24" t="s">
-        <v>122</v>
+        <v>185</v>
       </c>
       <c r="H75" s="15"/>
-      <c r="I75" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="J75" s="17"/>
     </row>
-    <row r="76" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H76" s="15"/>
-      <c r="J76" s="17"/>
-    </row>
+    <row r="76" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="77" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="17"/>
-      <c r="B77" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="H77" s="15"/>
-      <c r="I77" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="J77" s="17"/>
     </row>
-    <row r="78" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="17"/>
-      <c r="B78" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="H78" s="15"/>
-      <c r="I78" s="3" t="s">
-        <v>62</v>
-      </c>
+    <row r="78" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J78" s="17"/>
     </row>
     <row r="79" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="B79" s="12"/>
-      <c r="H79" s="15"/>
+      <c r="A79" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
       <c r="J79" s="17"/>
     </row>
     <row r="80" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="17"/>
       <c r="B80" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="H80" s="15" t="s">
-        <v>202</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H80" s="15"/>
       <c r="I80" s="3" t="s">
         <v>61</v>
       </c>
@@ -2443,101 +2302,55 @@
     <row r="81" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
       <c r="B81" s="24" t="s">
-        <v>203</v>
+        <v>168</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="H81" s="15"/>
+      <c r="I81" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J81" s="17"/>
     </row>
-    <row r="82" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="82" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="17"/>
+      <c r="B82" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H82" s="15"/>
+      <c r="I82" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J82" s="17"/>
+    </row>
     <row r="83" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="17"/>
+      <c r="B83" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H83" s="15"/>
+      <c r="I83" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J83" s="17"/>
     </row>
-    <row r="84" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J84" s="17"/>
-    </row>
-    <row r="85" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B85" s="14"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="14"/>
-      <c r="J85" s="17"/>
-    </row>
-    <row r="86" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="17"/>
-      <c r="B86" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H86" s="15"/>
-      <c r="I86" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J86" s="17"/>
-    </row>
-    <row r="87" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="17"/>
-      <c r="B87" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H87" s="15"/>
-      <c r="I87" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J87" s="17"/>
-    </row>
-    <row r="88" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="17"/>
-      <c r="B88" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H88" s="15"/>
-      <c r="I88" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J88" s="17"/>
-    </row>
-    <row r="89" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="17"/>
-      <c r="B89" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="H89" s="15"/>
-      <c r="I89" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J89" s="17"/>
-    </row>
-    <row r="90" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="84" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2546,10 +2359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD31"/>
+  <dimension ref="A1:AD57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" topLeftCell="M6" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,7 +2386,7 @@
     <col min="18" max="18" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2.85546875" style="4" customWidth="1"/>
     <col min="20" max="20" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="2.85546875" style="4" customWidth="1"/>
     <col min="23" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="2.85546875" style="4" customWidth="1"/>
@@ -2617,7 +2430,7 @@
       </c>
       <c r="O1" s="5"/>
       <c r="P1" s="1" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>60</v>
@@ -2655,7 +2468,7 @@
       </c>
     </row>
     <row r="2" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="N2" s="6"/>
+      <c r="N2" s="26"/>
       <c r="AD2" s="6"/>
     </row>
     <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2667,25 +2480,27 @@
         <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="1" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="H3" s="5"/>
       <c r="J3" s="20"/>
       <c r="K3" s="5"/>
       <c r="L3" s="20" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="N3" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="O3" s="5"/>
       <c r="S3" s="5"/>
       <c r="V3" s="5"/>
@@ -2699,7 +2514,7 @@
         <v>70</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
@@ -2722,7 +2537,7 @@
         <v>115</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
@@ -2741,7 +2556,7 @@
         <v>112</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
@@ -2760,7 +2575,7 @@
         <v>113</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
@@ -2873,20 +2688,22 @@
       <c r="M13" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="25"/>
+      <c r="N13" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="O13" s="5"/>
       <c r="P13" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q13" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S13" s="5"/>
+      <c r="T13" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="R13" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="S13" s="5"/>
-      <c r="T13" s="22" t="s">
-        <v>145</v>
       </c>
       <c r="U13" s="20"/>
       <c r="V13" s="5"/>
@@ -2925,18 +2742,9 @@
       </c>
       <c r="N14" s="25"/>
       <c r="O14" s="5"/>
-      <c r="P14" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q14" s="20" t="s">
+      <c r="S14" s="5"/>
+      <c r="T14" s="20" t="s">
         <v>88</v>
-      </c>
-      <c r="R14" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="S14" s="5"/>
-      <c r="T14" s="22" t="s">
-        <v>146</v>
       </c>
       <c r="U14" s="20"/>
       <c r="V14" s="5"/>
@@ -2975,18 +2783,9 @@
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q15" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="R15" s="22" t="s">
-        <v>142</v>
-      </c>
       <c r="S15" s="5"/>
-      <c r="T15" s="22" t="s">
-        <v>147</v>
+      <c r="T15" s="20" t="s">
+        <v>187</v>
       </c>
       <c r="U15" s="20"/>
       <c r="V15" s="5"/>
@@ -3014,18 +2813,9 @@
       <c r="M16" s="22"/>
       <c r="N16" s="25"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q16" s="20" t="s">
+      <c r="S16" s="5"/>
+      <c r="T16" s="20" t="s">
         <v>149</v>
-      </c>
-      <c r="R16" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="S16" s="5"/>
-      <c r="T16" s="22" t="s">
-        <v>132</v>
       </c>
       <c r="U16" s="20"/>
       <c r="V16" s="5"/>
@@ -3053,18 +2843,9 @@
       <c r="M17" s="20"/>
       <c r="N17" s="25"/>
       <c r="O17" s="5"/>
-      <c r="P17" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q17" s="20" t="s">
+      <c r="S17" s="5"/>
+      <c r="T17" s="20" t="s">
         <v>151</v>
-      </c>
-      <c r="R17" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="S17" s="5"/>
-      <c r="T17" s="22" t="s">
-        <v>133</v>
       </c>
       <c r="V17" s="5"/>
       <c r="Y17" s="5"/>
@@ -3090,15 +2871,9 @@
       <c r="K18" s="5"/>
       <c r="N18" s="6"/>
       <c r="O18" s="5"/>
-      <c r="Q18" s="20" t="s">
+      <c r="S18" s="5"/>
+      <c r="T18" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="R18" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="S18" s="5"/>
-      <c r="T18" s="22" t="s">
-        <v>182</v>
       </c>
       <c r="V18" s="5"/>
       <c r="Y18" s="5"/>
@@ -3127,7 +2902,7 @@
       <c r="AD19" s="6"/>
     </row>
     <row r="20" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="N20" s="6"/>
+      <c r="N20" s="26"/>
       <c r="AD20" s="6"/>
     </row>
     <row r="21" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3162,7 +2937,9 @@
       <c r="M21" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="N21" s="25"/>
+      <c r="N21" s="25" t="s">
+        <v>62</v>
+      </c>
       <c r="O21" s="5"/>
       <c r="P21" s="20" t="s">
         <v>111</v>
@@ -3203,7 +2980,7 @@
       <c r="AD22" s="6"/>
     </row>
     <row r="23" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="N23" s="6"/>
+      <c r="N23" s="26"/>
       <c r="AD23" s="6"/>
     </row>
     <row r="24" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3238,23 +3015,22 @@
       <c r="M24" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="N24" s="25"/>
+      <c r="N24" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="O24" s="5"/>
       <c r="P24" s="20" t="s">
-        <v>198</v>
+        <v>6</v>
       </c>
       <c r="Q24" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="R24" s="20" t="s">
-        <v>87</v>
+        <v>6</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="S24" s="21"/>
-      <c r="T24" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="U24" s="20" t="s">
-        <v>173</v>
+      <c r="T24" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="V24" s="5"/>
       <c r="Y24" s="5"/>
@@ -3293,20 +3069,14 @@
       <c r="N25" s="25"/>
       <c r="O25" s="5"/>
       <c r="P25" s="20" t="s">
-        <v>197</v>
+        <v>7</v>
       </c>
       <c r="Q25" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="R25" s="20" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="S25" s="5"/>
       <c r="T25" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="U25" s="20" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="V25" s="5"/>
       <c r="Y25" s="5"/>
@@ -3343,20 +3113,14 @@
       <c r="N26" s="25"/>
       <c r="O26" s="5"/>
       <c r="P26" s="20" t="s">
-        <v>196</v>
+        <v>14</v>
       </c>
       <c r="Q26" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="R26" s="20" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="S26" s="5"/>
       <c r="T26" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="U26" s="20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="V26" s="5"/>
       <c r="Y26" s="5"/>
@@ -3383,15 +3147,15 @@
       </c>
       <c r="N27" s="25"/>
       <c r="O27" s="5"/>
-      <c r="R27" s="1" t="s">
-        <v>155</v>
+      <c r="P27" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q27" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="S27" s="5"/>
       <c r="T27" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="U27" s="20" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="V27" s="5"/>
       <c r="Y27" s="5"/>
@@ -3413,16 +3177,7 @@
       <c r="L28" s="20"/>
       <c r="N28" s="6"/>
       <c r="O28" s="5"/>
-      <c r="R28" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="S28" s="5"/>
-      <c r="T28" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="U28" s="20" t="s">
-        <v>175</v>
-      </c>
       <c r="V28" s="5"/>
       <c r="Y28" s="5"/>
       <c r="AB28" s="5"/>
@@ -3443,16 +3198,7 @@
       <c r="L29" s="20"/>
       <c r="N29" s="6"/>
       <c r="O29" s="5"/>
-      <c r="R29" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="S29" s="5"/>
-      <c r="T29" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="U29" s="20" t="s">
-        <v>178</v>
-      </c>
       <c r="V29" s="5"/>
       <c r="Y29" s="5"/>
       <c r="AB29" s="5"/>
@@ -3482,8 +3228,173 @@
       <c r="AD30" s="6"/>
     </row>
     <row r="31" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="N31" s="6"/>
+      <c r="N31" s="26"/>
       <c r="AD31" s="6"/>
+    </row>
+    <row r="32" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="R32" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="T32" s="20"/>
+      <c r="U32" s="20"/>
+    </row>
+    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="R33" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="T33" s="20"/>
+      <c r="U33" s="20"/>
+    </row>
+    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="R34" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="T34" s="20"/>
+      <c r="U34" s="20"/>
+    </row>
+    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="R35" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="T35" s="20"/>
+      <c r="U35" s="20"/>
+    </row>
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="R36" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+    </row>
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="R37" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="T37" s="20"/>
+      <c r="U37" s="20"/>
+    </row>
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:21" s="27" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
+    </row>
+    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>193</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="R40" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="R41" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="R42" s="20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:21" s="27" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="26"/>
+    </row>
+    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T48" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="U48" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="20:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T49" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="U49" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="20:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T50" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="U50" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="51" spans="20:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T51" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="U51" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" spans="20:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T52" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="U52" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="20:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T53" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="U53" s="22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="20:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T54" s="22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="20:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T55" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="20:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T56" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="20:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T57" s="22" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Planning update + scene update
</commit_message>
<xml_diff>
--- a/Documentatie/Gamelab_2_Planning.xlsx
+++ b/Documentatie/Gamelab_2_Planning.xlsx
@@ -2362,7 +2362,7 @@
   <dimension ref="A1:AD57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M6" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+      <selection activeCell="T32" sqref="T32:T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3241,7 +3241,9 @@
       <c r="R32" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="T32" s="20"/>
+      <c r="T32" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="U32" s="20"/>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3249,7 +3251,9 @@
       <c r="R33" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="T33" s="20"/>
+      <c r="T33" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="U33" s="20"/>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3257,30 +3261,23 @@
       <c r="R34" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="T34" s="20"/>
+      <c r="T34" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="U34" s="20"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="R35" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="T35" s="20"/>
       <c r="U35" s="20"/>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="R36" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="T36" s="20"/>
       <c r="U36" s="20"/>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="R37" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="T37" s="20"/>
       <c r="U37" s="20"/>
     </row>

</xml_diff>